<commit_message>
Maj du context avec update domain afin d'avoir le même linspace à chaque fois !
</commit_message>
<xml_diff>
--- a/classes/Kernels/excel_test_unitaires_kernel.xlsx
+++ b/classes/Kernels/excel_test_unitaires_kernel.xlsx
@@ -1750,10 +1750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T149"/>
+  <dimension ref="A1:U149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="L96" sqref="L96"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="J110" sqref="J110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1765,12 +1765,12 @@
     <col min="6" max="6" width="2.83203125" customWidth="1"/>
     <col min="7" max="7" width="15.6640625" customWidth="1"/>
     <col min="8" max="11" width="15.5" customWidth="1"/>
-    <col min="12" max="12" width="27.6640625" style="6" customWidth="1"/>
-    <col min="13" max="15" width="15.6640625" customWidth="1"/>
-    <col min="16" max="16" width="18.1640625" customWidth="1"/>
+    <col min="12" max="13" width="27.6640625" style="6" customWidth="1"/>
+    <col min="14" max="16" width="15.6640625" customWidth="1"/>
+    <col min="17" max="17" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1798,20 +1798,20 @@
       <c r="L1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>38</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>49</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>42</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:21">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1845,24 +1845,25 @@
         <f>(D3*D3)/($E$3*4*H3)</f>
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="9"/>
+      <c r="N3">
         <f>G3^2</f>
         <v>4</v>
       </c>
-      <c r="N3">
-        <f>G3/O3</f>
+      <c r="O3">
+        <f>G3/P3</f>
         <v>0.57735026918962584</v>
       </c>
-      <c r="O3" s="5">
-        <f t="shared" ref="O3:O12" si="1">(3*M3/D3)^(1/2)</f>
+      <c r="P3" s="5">
+        <f t="shared" ref="P3:P12" si="1">(3*N3/D3)^(1/2)</f>
         <v>3.4641016151377544</v>
       </c>
-      <c r="P3" s="5">
-        <f t="shared" ref="P3:P12" si="2">(3/4)*((2*D3^(1/2))/(27^(1/2)*$E$3*M3^(1/2)))</f>
+      <c r="Q3" s="5">
+        <f t="shared" ref="Q3:Q12" si="2">(3/4)*((2*D3^(1/2))/(27^(1/2)*$E$3*N3^(1/2)))</f>
         <v>1.4433756729740644E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:21">
       <c r="A4">
         <v>2.62</v>
       </c>
@@ -1892,24 +1893,25 @@
         <f t="shared" ref="L4:L12" si="5">(D4*D4)/($E$3*4*H4)</f>
         <v>2.1645021645021644E-2</v>
       </c>
-      <c r="M4">
-        <f t="shared" ref="M4:M12" si="6">M3+G4^2</f>
+      <c r="M4" s="9"/>
+      <c r="N4">
+        <f t="shared" ref="N4:N12" si="6">N3+G4^2</f>
         <v>10.8644</v>
       </c>
-      <c r="N4">
-        <f t="shared" ref="N4:N12" si="7">G4/O4</f>
+      <c r="O4">
+        <f t="shared" ref="O4:O12" si="7">G4/P4</f>
         <v>0.64901209195749077</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <f t="shared" si="1"/>
         <v>4.0369047548833743</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <f t="shared" si="2"/>
         <v>1.2385726945753638E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:21">
       <c r="A5">
         <v>2.84</v>
       </c>
@@ -1939,24 +1941,25 @@
         <f t="shared" si="5"/>
         <v>3.0160857908847188E-2</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="9"/>
+      <c r="N5">
         <f t="shared" si="6"/>
         <v>18.93</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <f t="shared" si="7"/>
         <v>0.65274421729077803</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <f t="shared" si="1"/>
         <v>4.3508619835614182</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <f t="shared" si="2"/>
         <v>1.1491975656527782E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:21">
       <c r="A6">
         <v>2.95</v>
       </c>
@@ -1986,24 +1989,25 @@
         <f t="shared" si="5"/>
         <v>3.8424591738712779E-2</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="9"/>
+      <c r="N6">
         <f t="shared" si="6"/>
         <v>27.6325</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <f t="shared" si="7"/>
         <v>0.64800938382462836</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <f t="shared" si="1"/>
         <v>4.5524032114917068</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <f t="shared" si="2"/>
         <v>1.0983209895332684E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:21">
       <c r="A7">
         <v>4.3</v>
       </c>
@@ -2033,24 +2037,25 @@
         <f t="shared" si="5"/>
         <v>4.2488103331067298E-2</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="9"/>
+      <c r="N7">
         <f t="shared" si="6"/>
         <v>46.122500000000002</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <f t="shared" si="7"/>
         <v>0.81740334501982548</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <f t="shared" si="1"/>
         <v>5.2605608066060787</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <f t="shared" si="2"/>
         <v>9.5046900583700619E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:21">
       <c r="A8">
         <v>4.7</v>
       </c>
@@ -2080,24 +2085,25 @@
         <f t="shared" si="5"/>
         <v>4.6367851622874809E-2</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="9"/>
+      <c r="N8">
         <f t="shared" si="6"/>
         <v>68.212500000000006</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <f t="shared" si="7"/>
         <v>0.80478685158799235</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <f t="shared" si="1"/>
         <v>5.8400556504197807</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <f t="shared" si="2"/>
         <v>8.5615622509360879E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:21">
       <c r="A9">
         <v>4.97</v>
       </c>
@@ -2127,24 +2133,25 @@
         <f t="shared" si="5"/>
         <v>5.0246103363412634E-2</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="9"/>
+      <c r="N9">
         <f t="shared" si="6"/>
         <v>92.913399999999996</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <f t="shared" si="7"/>
         <v>0.78759981432374937</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <f t="shared" si="1"/>
         <v>6.3103112895821996</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <f t="shared" si="2"/>
         <v>7.9235393795145815E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:21">
       <c r="A10">
         <v>5.31</v>
       </c>
@@ -2174,24 +2181,25 @@
         <f t="shared" si="5"/>
         <v>5.3890198720107786E-2</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="9"/>
+      <c r="N10">
         <f t="shared" si="6"/>
         <v>121.1095</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <f t="shared" si="7"/>
         <v>0.78793389222151566</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <f t="shared" si="1"/>
         <v>6.739144048022716</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <f t="shared" si="2"/>
         <v>7.4193398514267022E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:21">
       <c r="A11">
         <v>5.7</v>
       </c>
@@ -2221,24 +2229,25 @@
         <f t="shared" si="5"/>
         <v>5.7219553546199495E-2</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="9"/>
+      <c r="N11">
         <f t="shared" si="6"/>
         <v>153.59950000000001</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <f t="shared" si="7"/>
         <v>0.79660051353567018</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <f t="shared" si="1"/>
         <v>7.1554058818024666</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <f t="shared" si="2"/>
         <v>6.987723802944476E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:21">
       <c r="A12">
         <v>7</v>
       </c>
@@ -2266,27 +2275,28 @@
       </c>
       <c r="K12" s="5"/>
       <c r="L12" s="8">
-        <f t="shared" si="5"/>
+        <f>(D12*D12)/($E$3*4*H12)</f>
         <v>5.8976173625855159E-2</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="9"/>
+      <c r="N12">
         <f t="shared" si="6"/>
         <v>202.59950000000001</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <f t="shared" si="7"/>
         <v>0.89787985559383099</v>
       </c>
-      <c r="O12" s="11">
+      <c r="P12" s="11">
         <f t="shared" si="1"/>
         <v>7.7961432772878156</v>
       </c>
-      <c r="P12" s="11">
+      <c r="Q12" s="11">
         <f t="shared" si="2"/>
         <v>6.4134275399559352E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:21">
       <c r="J13">
         <f>$B$16-$B$17</f>
         <v>1.5</v>
@@ -2294,26 +2304,26 @@
       <c r="L13" s="15">
         <v>0</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <f>$J$13</f>
         <v>1.5</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
         <v>47</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <f>15</f>
         <v>15</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>48</v>
       </c>
-      <c r="T13">
-        <f>10*(O13^3)</f>
+      <c r="U13">
+        <f>10*(P13^3)</f>
         <v>33.75</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:21">
       <c r="J14">
         <f>$B$16+$B$17</f>
         <v>2.5</v>
@@ -2322,26 +2332,26 @@
         <f>1/(J14*$E$3)-H3/($E$3*J14*J14)</f>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <f>$J$14</f>
         <v>2.5</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>47</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <f>25</f>
         <v>25</v>
       </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
         <v>48</v>
       </c>
-      <c r="T14">
-        <f>10*(O14^3)</f>
+      <c r="U14">
+        <f>10*(P14^3)</f>
         <v>156.25</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:21">
       <c r="G15" s="1" t="s">
         <v>4</v>
       </c>
@@ -2357,20 +2367,20 @@
       <c r="L15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>38</v>
       </c>
-      <c r="N15" t="s">
+      <c r="O15" t="s">
         <v>49</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
         <v>42</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:21">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -2379,7 +2389,7 @@
       </c>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:17">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -2406,24 +2416,25 @@
         <f t="shared" ref="L17:L26" si="11">(D3*D3)/($E$3*4*H17)</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="9"/>
+      <c r="N17">
         <f>G17^2</f>
         <v>1</v>
       </c>
-      <c r="N17">
-        <f>G17/O17</f>
+      <c r="O17">
+        <f>G17/P17</f>
         <v>0.57735026918962584</v>
       </c>
-      <c r="O17" s="5">
-        <f t="shared" ref="O17:O26" si="12">(3*M17/D3)^(1/2)</f>
+      <c r="P17" s="5">
+        <f t="shared" ref="P17:P26" si="12">(3*N17/D3)^(1/2)</f>
         <v>1.7320508075688772</v>
       </c>
-      <c r="P17" s="5">
-        <f t="shared" ref="P17:P26" si="13">(3/4)*((2*D3^(1/2))/(27^(1/2)*$E$3*M17^(1/2)))</f>
+      <c r="Q17" s="5">
+        <f t="shared" ref="Q17:Q26" si="13">(3/4)*((2*D3^(1/2))/(27^(1/2)*$E$3*N17^(1/2)))</f>
         <v>2.8867513459481287E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:17">
       <c r="C18" s="7"/>
       <c r="G18" s="2">
         <v>1.62</v>
@@ -2444,24 +2455,25 @@
         <f t="shared" si="11"/>
         <v>3.8167938931297704E-2</v>
       </c>
-      <c r="M18">
-        <f t="shared" ref="M18:M26" si="15">M17+G18^2</f>
+      <c r="M18" s="9"/>
+      <c r="N18">
+        <f t="shared" ref="N18:N26" si="15">N17+G18^2</f>
         <v>3.6244000000000005</v>
       </c>
-      <c r="N18">
-        <f t="shared" ref="N18:N26" si="16">G18/O18</f>
+      <c r="O18">
+        <f t="shared" ref="O18:O26" si="16">G18/P18</f>
         <v>0.69478642452054773</v>
       </c>
-      <c r="O18">
+      <c r="P18">
         <f t="shared" si="12"/>
         <v>2.331651775029882</v>
       </c>
-      <c r="P18">
+      <c r="Q18">
         <f t="shared" si="13"/>
         <v>2.1444025448165049E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:17">
       <c r="G19" s="2">
         <v>1.84</v>
       </c>
@@ -2481,24 +2493,25 @@
         <f t="shared" si="11"/>
         <v>5.0448430493273543E-2</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="9"/>
+      <c r="N19">
         <f t="shared" si="15"/>
         <v>7.0100000000000007</v>
       </c>
-      <c r="N19">
+      <c r="O19">
         <f t="shared" si="16"/>
         <v>0.69495840863245817</v>
       </c>
-      <c r="O19">
+      <c r="P19">
         <f t="shared" si="12"/>
         <v>2.6476404589747453</v>
       </c>
-      <c r="P19">
+      <c r="Q19">
         <f t="shared" si="13"/>
         <v>1.8884739365012448E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:17">
       <c r="G20" s="2">
         <v>1.95</v>
       </c>
@@ -2518,24 +2531,25 @@
         <f t="shared" si="11"/>
         <v>6.2402496099843996E-2</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="9"/>
+      <c r="N20">
         <f t="shared" si="15"/>
         <v>10.8125</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <f t="shared" si="16"/>
         <v>0.68476399883758943</v>
       </c>
-      <c r="O20">
+      <c r="P20">
         <f t="shared" si="12"/>
         <v>2.8476964374736293</v>
       </c>
-      <c r="P20">
+      <c r="Q20">
         <f t="shared" si="13"/>
         <v>1.7558051252245886E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:17">
       <c r="A21" s="11"/>
       <c r="B21" t="s">
         <v>44</v>
@@ -2559,24 +2573,25 @@
         <f t="shared" si="11"/>
         <v>6.4366632337796076E-2</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="9"/>
+      <c r="N21">
         <f t="shared" si="15"/>
         <v>21.702500000000001</v>
       </c>
-      <c r="N21">
+      <c r="O21">
         <f t="shared" si="16"/>
         <v>0.91449941551098557</v>
       </c>
-      <c r="O21">
+      <c r="P21">
         <f t="shared" si="12"/>
         <v>3.6085315572958483</v>
       </c>
-      <c r="P21">
+      <c r="Q21">
         <f t="shared" si="13"/>
         <v>1.3856051750166449E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:17">
       <c r="G22" s="4">
         <v>3.7</v>
       </c>
@@ -2596,24 +2611,25 @@
         <f t="shared" si="11"/>
         <v>6.7114093959731544E-2</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="9"/>
+      <c r="N22">
         <f t="shared" si="15"/>
         <v>35.392499999999998</v>
       </c>
-      <c r="N22">
+      <c r="O22">
         <f t="shared" si="16"/>
         <v>0.87955115152882535</v>
       </c>
-      <c r="O22">
+      <c r="P22">
         <f t="shared" si="12"/>
         <v>4.2066910987140478</v>
       </c>
-      <c r="P22">
+      <c r="Q22">
         <f t="shared" si="13"/>
         <v>1.1885826372011153E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:17">
       <c r="A23" s="5"/>
       <c r="B23" t="s">
         <v>40</v>
@@ -2637,24 +2653,25 @@
         <f t="shared" si="11"/>
         <v>7.0483314154200241E-2</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="9"/>
+      <c r="N23">
         <f t="shared" si="15"/>
         <v>51.153399999999998</v>
       </c>
-      <c r="N23">
+      <c r="O23">
         <f t="shared" si="16"/>
         <v>0.84789416552605279</v>
       </c>
-      <c r="O23">
+      <c r="P23">
         <f t="shared" si="12"/>
         <v>4.6821881331580126</v>
       </c>
-      <c r="P23">
+      <c r="Q23">
         <f t="shared" si="13"/>
         <v>1.067876782778404E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:17">
       <c r="G24" s="4">
         <v>4.3099999999999996</v>
       </c>
@@ -2674,24 +2691,25 @@
         <f t="shared" si="11"/>
         <v>7.376671277086215E-2</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="9"/>
+      <c r="N24">
         <f t="shared" si="15"/>
         <v>69.729500000000002</v>
       </c>
-      <c r="N24">
+      <c r="O24">
         <f t="shared" si="16"/>
         <v>0.84285595731111262</v>
       </c>
-      <c r="O24">
+      <c r="P24">
         <f t="shared" si="12"/>
         <v>5.1135665146744698</v>
       </c>
-      <c r="P24">
+      <c r="Q24">
         <f t="shared" si="13"/>
         <v>9.7779113377159249E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:17">
       <c r="A25" s="15"/>
       <c r="B25" t="s">
         <v>45</v>
@@ -2715,24 +2733,25 @@
         <f t="shared" si="11"/>
         <v>7.6733611216369846E-2</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="9"/>
+      <c r="N25">
         <f t="shared" si="15"/>
         <v>91.819500000000005</v>
       </c>
-      <c r="N25">
+      <c r="O25">
         <f t="shared" si="16"/>
         <v>0.84955406749854334</v>
       </c>
-      <c r="O25">
+      <c r="P25">
         <f t="shared" si="12"/>
         <v>5.5323141631689721</v>
       </c>
-      <c r="P25">
+      <c r="Q25">
         <f t="shared" si="13"/>
         <v>9.0378092287079076E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:17">
       <c r="G26" s="4">
         <v>6</v>
       </c>
@@ -2753,24 +2772,25 @@
         <f t="shared" si="11"/>
         <v>7.7184316146958948E-2</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="9"/>
+      <c r="N26">
         <f t="shared" si="15"/>
         <v>127.81950000000001</v>
       </c>
-      <c r="N26">
+      <c r="O26">
         <f t="shared" si="16"/>
         <v>0.96892924838392602</v>
       </c>
-      <c r="O26" s="11">
+      <c r="P26" s="11">
         <f t="shared" si="12"/>
         <v>6.1924026031904607</v>
       </c>
-      <c r="P26" s="11">
+      <c r="Q26" s="11">
         <f t="shared" si="13"/>
         <v>8.0744104031993825E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:17">
       <c r="A27" s="16"/>
       <c r="B27" t="s">
         <v>46</v>
@@ -2783,12 +2803,12 @@
         <f>1/(J27*$E$3)-H17/($E$3*J27*J27)</f>
         <v>2.222222222222222E-2</v>
       </c>
-      <c r="O27">
+      <c r="P27">
         <f>$J$13</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:17">
       <c r="J28">
         <f>$J$14</f>
         <v>2.5</v>
@@ -2797,12 +2817,12 @@
         <f>4/(J28*$E$3)-H20/($E$3*J28*J28)</f>
         <v>5.7440000000000005E-2</v>
       </c>
-      <c r="O28">
+      <c r="P28">
         <f>$J$14</f>
         <v>2.5</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:17">
       <c r="G30" t="s">
         <v>5</v>
       </c>
@@ -2818,20 +2838,20 @@
       <c r="L30" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="M30" t="s">
+      <c r="N30" t="s">
         <v>38</v>
       </c>
-      <c r="N30" t="s">
+      <c r="O30" t="s">
         <v>49</v>
       </c>
-      <c r="O30" t="s">
+      <c r="P30" t="s">
         <v>42</v>
       </c>
-      <c r="P30" t="s">
+      <c r="Q30" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:17">
       <c r="G32">
         <f t="shared" ref="G32:G41" si="18">ABS($C$5-A3)</f>
         <v>0</v>
@@ -2852,24 +2872,25 @@
         <f t="shared" ref="L32:L41" si="20">(D3*D3)/($E$3*4*H32)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M32">
+      <c r="M32" s="9"/>
+      <c r="N32">
         <f>G32^2</f>
         <v>0</v>
       </c>
-      <c r="N32" t="e">
-        <f>G32/O32</f>
+      <c r="O32" t="e">
+        <f>G32/P32</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O32">
-        <f t="shared" ref="O32:O41" si="21">(3*M32/D3)^(1/2)</f>
+      <c r="P32">
+        <f t="shared" ref="P32:P41" si="21">(3*N32/D3)^(1/2)</f>
         <v>0</v>
       </c>
-      <c r="P32" t="e">
-        <f t="shared" ref="P32:P41" si="22">(3/4)*((2*D3^(1/2))/(27^(1/2)*$E$3*M32^(1/2)))</f>
+      <c r="Q32" t="e">
+        <f t="shared" ref="Q32:Q41" si="22">(3/4)*((2*D3^(1/2))/(27^(1/2)*$E$3*N32^(1/2)))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="7:16">
+    <row r="33" spans="7:17">
       <c r="G33">
         <f t="shared" si="18"/>
         <v>0.62000000000000011</v>
@@ -2891,24 +2912,25 @@
         <f t="shared" si="20"/>
         <v>0.16129032258064513</v>
       </c>
-      <c r="M33">
-        <f t="shared" ref="M33:M41" si="24">M32+G33^2</f>
+      <c r="M33" s="9"/>
+      <c r="N33">
+        <f t="shared" ref="N33:N41" si="24">N32+G33^2</f>
         <v>0.38440000000000013</v>
       </c>
-      <c r="N33">
-        <f t="shared" ref="N33:N41" si="25">G33/O33</f>
+      <c r="O33">
+        <f t="shared" ref="O33:O41" si="25">G33/P33</f>
         <v>0.81649658092772592</v>
       </c>
-      <c r="O33" s="5">
+      <c r="P33" s="5">
         <f t="shared" si="21"/>
         <v>0.75934182026278541</v>
       </c>
-      <c r="P33" s="5">
+      <c r="Q33" s="5">
         <f t="shared" si="22"/>
         <v>6.5846498461913372E-2</v>
       </c>
     </row>
-    <row r="34" spans="7:16">
+    <row r="34" spans="7:17">
       <c r="G34">
         <f t="shared" si="18"/>
         <v>0.83999999999999986</v>
@@ -2929,24 +2951,25 @@
         <f t="shared" si="20"/>
         <v>0.1541095890410959</v>
       </c>
-      <c r="M34">
+      <c r="M34" s="9"/>
+      <c r="N34">
         <f t="shared" si="24"/>
         <v>1.0899999999999999</v>
       </c>
-      <c r="N34">
+      <c r="O34">
         <f t="shared" si="25"/>
         <v>0.80457407958576721</v>
       </c>
-      <c r="O34">
+      <c r="P34">
         <f t="shared" si="21"/>
         <v>1.0440306508910548</v>
       </c>
-      <c r="P34">
+      <c r="Q34">
         <f t="shared" si="22"/>
         <v>4.7891314261057576E-2</v>
       </c>
     </row>
-    <row r="35" spans="7:16">
+    <row r="35" spans="7:17">
       <c r="G35">
         <f t="shared" si="18"/>
         <v>0.95000000000000018</v>
@@ -2968,24 +2991,25 @@
         <f t="shared" si="20"/>
         <v>0.16597510373443983</v>
       </c>
-      <c r="M35">
+      <c r="M35" s="9"/>
+      <c r="N35">
         <f t="shared" si="24"/>
         <v>1.9925000000000002</v>
       </c>
-      <c r="N35">
+      <c r="O35">
         <f t="shared" si="25"/>
         <v>0.77713023969738326</v>
       </c>
-      <c r="O35">
+      <c r="P35">
         <f t="shared" si="21"/>
         <v>1.2224463178397651</v>
       </c>
-      <c r="P35">
+      <c r="Q35">
         <f t="shared" si="22"/>
         <v>4.0901591563020152E-2</v>
       </c>
     </row>
-    <row r="36" spans="7:16">
+    <row r="36" spans="7:17">
       <c r="G36">
         <f t="shared" si="18"/>
         <v>2.2999999999999998</v>
@@ -3010,24 +3034,25 @@
         <f t="shared" si="20"/>
         <v>0.1326963906581741</v>
       </c>
-      <c r="M36">
+      <c r="M36" s="9"/>
+      <c r="N36">
         <f t="shared" si="24"/>
         <v>7.2824999999999989</v>
       </c>
-      <c r="N36" s="21">
+      <c r="O36" s="21">
         <f t="shared" si="25"/>
         <v>1.1003021565886204</v>
       </c>
-      <c r="O36" s="21">
+      <c r="P36" s="21">
         <f t="shared" si="21"/>
         <v>2.0903349013973811</v>
       </c>
-      <c r="P36" s="21">
+      <c r="Q36" s="21">
         <f t="shared" si="22"/>
         <v>2.3919612099752616E-2</v>
       </c>
     </row>
-    <row r="37" spans="7:16">
+    <row r="37" spans="7:17">
       <c r="G37">
         <f t="shared" si="18"/>
         <v>2.7</v>
@@ -3049,24 +3074,25 @@
         <f t="shared" si="20"/>
         <v>0.12145748987854252</v>
       </c>
-      <c r="M37">
+      <c r="M37" s="9"/>
+      <c r="N37">
         <f t="shared" si="24"/>
         <v>14.5725</v>
       </c>
-      <c r="N37" s="21">
+      <c r="O37" s="21">
         <f t="shared" si="25"/>
         <v>1.0002573009176763</v>
       </c>
-      <c r="O37" s="21">
+      <c r="P37" s="21">
         <f t="shared" si="21"/>
         <v>2.6993054662264515</v>
       </c>
-      <c r="P37" s="21">
+      <c r="Q37" s="21">
         <f t="shared" si="22"/>
         <v>1.8523283350327335E-2</v>
       </c>
     </row>
-    <row r="38" spans="7:16">
+    <row r="38" spans="7:17">
       <c r="G38">
         <f t="shared" si="18"/>
         <v>2.9699999999999998</v>
@@ -3088,24 +3114,25 @@
         <f t="shared" si="20"/>
         <v>0.11801541425818884</v>
       </c>
-      <c r="M38">
+      <c r="M38" s="9"/>
+      <c r="N38">
         <f t="shared" si="24"/>
         <v>23.3934</v>
       </c>
-      <c r="N38">
+      <c r="O38">
         <f t="shared" si="25"/>
         <v>0.93798991405472942</v>
       </c>
-      <c r="O38">
+      <c r="P38">
         <f t="shared" si="21"/>
         <v>3.1663453471064802</v>
       </c>
-      <c r="P38">
+      <c r="Q38">
         <f t="shared" si="22"/>
         <v>1.5791075994187366E-2</v>
       </c>
     </row>
-    <row r="39" spans="7:16">
+    <row r="39" spans="7:17">
       <c r="G39">
         <f t="shared" si="18"/>
         <v>3.3099999999999996</v>
@@ -3126,24 +3153,25 @@
         <f t="shared" si="20"/>
         <v>0.11687363038714392</v>
       </c>
-      <c r="M39">
+      <c r="M39" s="9"/>
+      <c r="N39">
         <f t="shared" si="24"/>
         <v>34.349499999999999</v>
       </c>
-      <c r="N39">
+      <c r="O39">
         <f t="shared" si="25"/>
         <v>0.92225740305898374</v>
       </c>
-      <c r="O39">
+      <c r="P39">
         <f t="shared" si="21"/>
         <v>3.5890197129578429</v>
       </c>
-      <c r="P39">
+      <c r="Q39">
         <f t="shared" si="22"/>
         <v>1.3931380710860782E-2</v>
       </c>
     </row>
-    <row r="40" spans="7:16">
+    <row r="40" spans="7:17">
       <c r="G40">
         <f t="shared" si="18"/>
         <v>3.7</v>
@@ -3165,24 +3193,25 @@
         <f t="shared" si="20"/>
         <v>0.11644623346751008</v>
       </c>
-      <c r="M40">
+      <c r="M40" s="9"/>
+      <c r="N40">
         <f t="shared" si="24"/>
         <v>48.039500000000004</v>
       </c>
-      <c r="N40">
+      <c r="O40">
         <f t="shared" si="25"/>
         <v>0.92461963578161566</v>
       </c>
-      <c r="O40" s="11">
+      <c r="P40" s="11">
         <f t="shared" si="21"/>
         <v>4.0016454948766595</v>
       </c>
-      <c r="P40" s="11">
+      <c r="Q40" s="11">
         <f t="shared" si="22"/>
         <v>1.2494859942994804E-2</v>
       </c>
     </row>
-    <row r="41" spans="7:16">
+    <row r="41" spans="7:17">
       <c r="G41">
         <f t="shared" si="18"/>
         <v>5</v>
@@ -3204,24 +3233,25 @@
         <f t="shared" si="20"/>
         <v>0.11165698972755696</v>
       </c>
-      <c r="M41">
+      <c r="M41" s="9"/>
+      <c r="N41">
         <f t="shared" si="24"/>
         <v>73.039500000000004</v>
       </c>
-      <c r="N41" s="21">
+      <c r="O41" s="21">
         <f t="shared" si="25"/>
         <v>1.0681456623941037</v>
       </c>
-      <c r="O41" s="21">
+      <c r="P41" s="21">
         <f t="shared" si="21"/>
         <v>4.6810095065060491</v>
       </c>
-      <c r="P41" s="21">
+      <c r="Q41" s="21">
         <f t="shared" si="22"/>
         <v>1.0681456623941038E-2</v>
       </c>
     </row>
-    <row r="42" spans="7:16">
+    <row r="42" spans="7:17">
       <c r="J42" s="16">
         <f>$J$13</f>
         <v>1.5</v>
@@ -3231,12 +3261,13 @@
         <f>4/(10*J42)-H35/(10*J42*J42)</f>
         <v>0.15955555555555556</v>
       </c>
-      <c r="O42">
+      <c r="M42" s="9"/>
+      <c r="P42">
         <f>$J$13</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="43" spans="7:16">
+    <row r="43" spans="7:17">
       <c r="J43" s="15">
         <f>$J$14</f>
         <v>2.5</v>
@@ -3246,12 +3277,13 @@
         <f>5/(10*2.5)-H36/(10*2.5*2.5)</f>
         <v>0.12464000000000001</v>
       </c>
-      <c r="O43">
+      <c r="M43" s="9"/>
+      <c r="P43">
         <f>$J$14</f>
         <v>2.5</v>
       </c>
     </row>
-    <row r="45" spans="7:16">
+    <row r="45" spans="7:17">
       <c r="G45" t="s">
         <v>6</v>
       </c>
@@ -3267,403 +3299,412 @@
       <c r="L45" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="M45" t="s">
+      <c r="N45" t="s">
         <v>38</v>
       </c>
-      <c r="N45" t="s">
+      <c r="O45" t="s">
         <v>49</v>
       </c>
-      <c r="O45" t="s">
+      <c r="P45" t="s">
         <v>42</v>
       </c>
-      <c r="P45" t="s">
+      <c r="Q45" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="7:16">
+    <row r="46" spans="7:17">
       <c r="L46"/>
     </row>
-    <row r="47" spans="7:16">
+    <row r="47" spans="7:17">
       <c r="G47">
-        <v>0.16</v>
+        <v>0.05</v>
       </c>
       <c r="H47">
         <f>G47</f>
-        <v>0.16</v>
-      </c>
-      <c r="I47">
+        <v>0.05</v>
+      </c>
+      <c r="I47" s="5">
         <f>G47/J47</f>
         <v>0.5</v>
       </c>
-      <c r="J47" s="11">
+      <c r="J47" s="5">
         <f t="shared" ref="J47:J56" si="27">2*H47/D3</f>
-        <v>0.32</v>
-      </c>
-      <c r="K47" s="11"/>
-      <c r="L47" s="12">
+        <v>0.1</v>
+      </c>
+      <c r="K47" s="5"/>
+      <c r="L47" s="8">
         <f t="shared" ref="L47:L56" si="28">(D3*D3)/($E$3*4*H47)</f>
-        <v>0.15625</v>
-      </c>
-      <c r="M47">
+        <v>0.5</v>
+      </c>
+      <c r="M47" s="9"/>
+      <c r="N47">
         <f>G47^2</f>
-        <v>2.5600000000000001E-2</v>
-      </c>
-      <c r="N47">
-        <f>G47/O47</f>
+        <v>2.5000000000000005E-3</v>
+      </c>
+      <c r="O47">
+        <f>G47/P47</f>
         <v>0.57735026918962573</v>
       </c>
-      <c r="O47" s="5">
-        <f t="shared" ref="O47:O56" si="29">(3*M47/D3)^(1/2)</f>
-        <v>0.27712812921102037</v>
-      </c>
       <c r="P47" s="5">
-        <f t="shared" ref="P47:P56" si="30">(3/4)*((2*D3^(1/2))/(27^(1/2)*$E$3*M47^(1/2)))</f>
-        <v>0.18042195912175801</v>
-      </c>
-    </row>
-    <row r="48" spans="7:16">
+        <f t="shared" ref="P47:P56" si="29">(3*N47/D3)^(1/2)</f>
+        <v>8.6602540378443879E-2</v>
+      </c>
+      <c r="Q47" s="5">
+        <f t="shared" ref="Q47:Q56" si="30">(3/4)*((2*D3^(1/2))/(27^(1/2)*$E$3*N47^(1/2)))</f>
+        <v>0.57735026918962573</v>
+      </c>
+    </row>
+    <row r="48" spans="7:17">
       <c r="G48">
-        <f>ABS($C$6-A4)</f>
-        <v>0.37999999999999989</v>
+        <v>0.16</v>
       </c>
       <c r="H48">
         <f>H47+G48</f>
-        <v>0.53999999999999992</v>
+        <v>0.21000000000000002</v>
       </c>
       <c r="I48">
         <f t="shared" ref="I48:I56" si="31">G48/J48</f>
-        <v>0.70370370370370361</v>
+        <v>0.76190476190476186</v>
       </c>
       <c r="J48">
         <f t="shared" si="27"/>
-        <v>0.53999999999999992</v>
+        <v>0.21000000000000002</v>
       </c>
       <c r="L48" s="9">
         <f t="shared" si="28"/>
-        <v>0.1851851851851852</v>
-      </c>
-      <c r="M48">
-        <f t="shared" ref="M48:M56" si="32">M47+G48^2</f>
-        <v>0.16999999999999993</v>
-      </c>
+        <v>0.47619047619047616</v>
+      </c>
+      <c r="M48" s="9"/>
       <c r="N48">
-        <f t="shared" ref="N48:N56" si="33">G48/O48</f>
-        <v>0.75251213266227235</v>
+        <f t="shared" ref="N48:N56" si="32">N47+G48^2</f>
+        <v>2.81E-2</v>
       </c>
       <c r="O48">
+        <f t="shared" ref="O48:O56" si="33">G48/P48</f>
+        <v>0.77932963862957283</v>
+      </c>
+      <c r="P48">
         <f t="shared" si="29"/>
-        <v>0.5049752469181038</v>
-      </c>
-      <c r="P48">
+        <v>0.2053046516764781</v>
+      </c>
+      <c r="Q48">
         <f t="shared" si="30"/>
-        <v>9.9014754297667457E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="7:16">
+        <v>0.24354051207174152</v>
+      </c>
+    </row>
+    <row r="49" spans="7:17">
       <c r="G49">
         <v>0.38</v>
       </c>
       <c r="H49">
         <f t="shared" ref="H49:H56" si="34">H48+G49</f>
-        <v>0.91999999999999993</v>
+        <v>0.59000000000000008</v>
       </c>
       <c r="I49">
         <f t="shared" si="31"/>
-        <v>0.61956521739130443</v>
-      </c>
-      <c r="J49" s="5">
+        <v>0.96610169491525422</v>
+      </c>
+      <c r="J49" s="6">
         <f t="shared" si="27"/>
-        <v>0.61333333333333329</v>
-      </c>
-      <c r="K49" s="5"/>
-      <c r="L49" s="8">
+        <v>0.39333333333333337</v>
+      </c>
+      <c r="K49" s="6"/>
+      <c r="L49" s="9">
         <f t="shared" si="28"/>
-        <v>0.24456521739130438</v>
-      </c>
-      <c r="M49">
+        <v>0.38135593220338981</v>
+      </c>
+      <c r="M49" s="9"/>
+      <c r="N49">
         <f t="shared" si="32"/>
-        <v>0.3143999999999999</v>
-      </c>
-      <c r="N49">
+        <v>0.17249999999999999</v>
+      </c>
+      <c r="O49">
         <f t="shared" si="33"/>
-        <v>0.6777075562561008</v>
-      </c>
-      <c r="O49">
+        <v>0.91493248345184597</v>
+      </c>
+      <c r="P49">
         <f t="shared" si="29"/>
-        <v>0.56071383075504733</v>
-      </c>
-      <c r="P49">
+        <v>0.41533119314590372</v>
+      </c>
+      <c r="Q49">
         <f t="shared" si="30"/>
-        <v>8.9172046875802727E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="7:16">
+        <v>0.1203858530857692</v>
+      </c>
+    </row>
+    <row r="50" spans="7:17">
       <c r="G50">
         <v>1</v>
       </c>
       <c r="H50">
         <f t="shared" si="34"/>
-        <v>1.92</v>
+        <v>1.59</v>
       </c>
       <c r="I50" s="21">
         <f t="shared" si="31"/>
-        <v>1.0416666666666667</v>
+        <v>1.2578616352201257</v>
       </c>
       <c r="J50" s="21">
         <f t="shared" si="27"/>
-        <v>0.96</v>
+        <v>0.79500000000000004</v>
       </c>
       <c r="K50" s="21"/>
       <c r="L50" s="22">
         <f t="shared" si="28"/>
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="M50">
+        <v>0.25157232704402516</v>
+      </c>
+      <c r="M50" s="9"/>
+      <c r="N50">
         <f t="shared" si="32"/>
-        <v>1.3144</v>
-      </c>
-      <c r="N50" s="21">
+        <v>1.1724999999999999</v>
+      </c>
+      <c r="O50" s="21">
         <f t="shared" si="33"/>
-        <v>1.0071765210390677</v>
-      </c>
-      <c r="O50" s="21">
+        <v>1.0663823359494558</v>
+      </c>
+      <c r="P50" s="21">
         <f t="shared" si="29"/>
-        <v>0.99287461444031289</v>
-      </c>
-      <c r="P50" s="21">
+        <v>0.93774996667555255</v>
+      </c>
+      <c r="Q50" s="21">
         <f t="shared" si="30"/>
-        <v>5.0358826051953381E-2</v>
-      </c>
-    </row>
-    <row r="51" spans="7:16">
+        <v>5.3319116797472789E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="7:17">
       <c r="G51">
         <v>1.3</v>
       </c>
       <c r="H51">
         <f t="shared" si="34"/>
-        <v>3.2199999999999998</v>
+        <v>2.89</v>
       </c>
       <c r="I51" s="21">
         <f t="shared" si="31"/>
-        <v>1.0093167701863355</v>
+        <v>1.1245674740484428</v>
       </c>
       <c r="J51" s="21">
         <f t="shared" si="27"/>
-        <v>1.2879999999999998</v>
+        <v>1.1560000000000001</v>
       </c>
       <c r="K51" s="21"/>
       <c r="L51" s="22">
         <f t="shared" si="28"/>
-        <v>0.19409937888198761</v>
-      </c>
-      <c r="M51">
+        <v>0.2162629757785467</v>
+      </c>
+      <c r="M51" s="9"/>
+      <c r="N51">
         <f t="shared" si="32"/>
-        <v>3.0044000000000004</v>
-      </c>
-      <c r="N51">
+        <v>2.8624999999999998</v>
+      </c>
+      <c r="O51">
         <f t="shared" si="33"/>
-        <v>0.96825299821294186</v>
-      </c>
-      <c r="O51">
+        <v>0.99196187183147044</v>
+      </c>
+      <c r="P51">
         <f t="shared" si="29"/>
-        <v>1.342624295921983</v>
-      </c>
-      <c r="P51">
+        <v>1.3105342422081157</v>
+      </c>
+      <c r="Q51">
         <f t="shared" si="30"/>
-        <v>3.724049993126699E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="7:16">
+        <v>3.8152379685825785E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="7:17">
       <c r="G52">
         <v>1.7</v>
       </c>
       <c r="H52">
         <f t="shared" si="34"/>
-        <v>4.92</v>
+        <v>4.59</v>
       </c>
       <c r="I52" s="21">
         <f t="shared" si="31"/>
-        <v>1.0365853658536586</v>
+        <v>1.1111111111111112</v>
       </c>
       <c r="J52" s="21">
         <f t="shared" si="27"/>
-        <v>1.64</v>
+        <v>1.53</v>
       </c>
       <c r="K52" s="21"/>
       <c r="L52" s="22">
         <f t="shared" si="28"/>
-        <v>0.18292682926829268</v>
-      </c>
-      <c r="M52">
+        <v>0.19607843137254902</v>
+      </c>
+      <c r="M52" s="9"/>
+      <c r="N52">
         <f t="shared" si="32"/>
-        <v>5.8944000000000001</v>
-      </c>
-      <c r="N52">
+        <v>5.7524999999999995</v>
+      </c>
+      <c r="O52">
         <f t="shared" si="33"/>
-        <v>0.99024832648174244</v>
-      </c>
-      <c r="O52">
+        <v>1.0023874152263978</v>
+      </c>
+      <c r="P52">
         <f t="shared" si="29"/>
-        <v>1.7167410987099947</v>
-      </c>
-      <c r="P52">
+        <v>1.6959510606146631</v>
+      </c>
+      <c r="Q52">
         <f t="shared" si="30"/>
-        <v>2.912495077887477E-2</v>
-      </c>
-    </row>
-    <row r="53" spans="7:16">
+        <v>2.9481982800776407E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="7:17">
       <c r="G53">
         <v>1.97</v>
       </c>
       <c r="H53">
         <f t="shared" si="34"/>
-        <v>6.89</v>
+        <v>6.56</v>
       </c>
       <c r="I53" s="21">
         <f t="shared" si="31"/>
-        <v>1.0007256894049348</v>
+        <v>1.0510670731707319</v>
       </c>
       <c r="J53" s="21">
         <f t="shared" si="27"/>
-        <v>1.9685714285714284</v>
+        <v>1.8742857142857141</v>
       </c>
       <c r="K53" s="21"/>
       <c r="L53" s="22">
         <f t="shared" si="28"/>
-        <v>0.17779390420899857</v>
-      </c>
-      <c r="M53">
+        <v>0.18673780487804881</v>
+      </c>
+      <c r="M53" s="9"/>
+      <c r="N53">
         <f t="shared" si="32"/>
-        <v>9.7752999999999997</v>
-      </c>
-      <c r="N53">
+        <v>9.6334</v>
+      </c>
+      <c r="O53">
         <f t="shared" si="33"/>
-        <v>0.96247525232076314</v>
-      </c>
-      <c r="O53">
+        <v>0.9695379700690977</v>
+      </c>
+      <c r="P53">
         <f t="shared" si="29"/>
-        <v>2.0468058739690691</v>
-      </c>
-      <c r="P53">
+        <v>2.0318956666128307</v>
+      </c>
+      <c r="Q53">
         <f t="shared" si="30"/>
-        <v>2.4428305896466065E-2</v>
-      </c>
-    </row>
-    <row r="54" spans="7:16">
+        <v>2.4607562692109078E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="7:17">
       <c r="G54">
         <v>2.31</v>
       </c>
       <c r="H54">
         <f t="shared" si="34"/>
-        <v>9.1999999999999993</v>
+        <v>8.8699999999999992</v>
       </c>
       <c r="I54" s="21">
         <f t="shared" si="31"/>
-        <v>1.0043478260869567</v>
+        <v>1.0417136414881625</v>
       </c>
       <c r="J54" s="21">
         <f t="shared" si="27"/>
-        <v>2.2999999999999998</v>
+        <v>2.2174999999999998</v>
       </c>
       <c r="K54" s="21"/>
       <c r="L54" s="22">
         <f t="shared" si="28"/>
-        <v>0.17391304347826086</v>
-      </c>
-      <c r="M54">
+        <v>0.18038331454340475</v>
+      </c>
+      <c r="M54" s="9"/>
+      <c r="N54">
         <f t="shared" si="32"/>
-        <v>15.1114</v>
-      </c>
-      <c r="N54">
+        <v>14.9695</v>
+      </c>
+      <c r="O54">
         <f t="shared" si="33"/>
-        <v>0.97038482253846881</v>
-      </c>
-      <c r="O54">
+        <v>0.97497324651699813</v>
+      </c>
+      <c r="P54">
         <f t="shared" si="29"/>
-        <v>2.3804988972902295</v>
-      </c>
-      <c r="P54">
+        <v>2.3692957814506825</v>
+      </c>
+      <c r="Q54">
         <f t="shared" si="30"/>
-        <v>2.1004000487845641E-2</v>
-      </c>
-    </row>
-    <row r="55" spans="7:16">
+        <v>2.1103317024177452E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="7:17">
       <c r="G55">
         <v>2.7</v>
       </c>
       <c r="H55">
         <f t="shared" si="34"/>
-        <v>11.899999999999999</v>
+        <v>11.57</v>
       </c>
       <c r="I55" s="21">
         <f t="shared" si="31"/>
-        <v>1.0210084033613449</v>
+        <v>1.0501296456352638</v>
       </c>
       <c r="J55" s="21">
         <f t="shared" si="27"/>
-        <v>2.6444444444444439</v>
+        <v>2.5711111111111111</v>
       </c>
       <c r="K55" s="21"/>
       <c r="L55" s="22">
         <f t="shared" si="28"/>
-        <v>0.17016806722689079</v>
-      </c>
-      <c r="M55">
+        <v>0.17502160760587726</v>
+      </c>
+      <c r="M55" s="9"/>
+      <c r="N55">
         <f t="shared" si="32"/>
-        <v>22.401400000000002</v>
-      </c>
-      <c r="N55">
+        <v>22.259500000000003</v>
+      </c>
+      <c r="O55">
         <f t="shared" si="33"/>
-        <v>0.9880679472194791</v>
-      </c>
-      <c r="O55" s="11">
+        <v>0.99121231486566763</v>
+      </c>
+      <c r="P55" s="11">
         <f t="shared" si="29"/>
-        <v>2.7326055941780796</v>
-      </c>
-      <c r="P55" s="11">
+        <v>2.7239371015743616</v>
+      </c>
+      <c r="Q55" s="11">
         <f t="shared" si="30"/>
-        <v>1.8297554578138503E-2</v>
-      </c>
-    </row>
-    <row r="56" spans="7:16">
+        <v>1.8355783608623472E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="7:17">
       <c r="G56">
         <v>4</v>
       </c>
       <c r="H56">
         <f t="shared" si="34"/>
-        <v>15.899999999999999</v>
+        <v>15.57</v>
       </c>
       <c r="I56" s="21">
         <f t="shared" si="31"/>
-        <v>1.257861635220126</v>
+        <v>1.2845215157353886</v>
       </c>
       <c r="J56" s="21">
         <f t="shared" si="27"/>
-        <v>3.1799999999999997</v>
+        <v>3.1139999999999999</v>
       </c>
       <c r="K56" s="21"/>
       <c r="L56" s="22">
         <f t="shared" si="28"/>
-        <v>0.15723270440251572</v>
-      </c>
-      <c r="M56">
+        <v>0.16056518946692358</v>
+      </c>
+      <c r="M56" s="9"/>
+      <c r="N56">
         <f t="shared" si="32"/>
-        <v>38.401400000000002</v>
-      </c>
-      <c r="N56" s="21">
+        <v>38.259500000000003</v>
+      </c>
+      <c r="O56" s="21">
         <f t="shared" si="33"/>
-        <v>1.1784898192860525</v>
-      </c>
-      <c r="O56" s="21">
+        <v>1.1806732369371924</v>
+      </c>
+      <c r="P56" s="21">
         <f t="shared" si="29"/>
-        <v>3.3941744209748563</v>
-      </c>
-      <c r="P56" s="21">
+        <v>3.3878975781448886</v>
+      </c>
+      <c r="Q56" s="21">
         <f t="shared" si="30"/>
-        <v>1.4731122741075655E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="7:16">
+        <v>1.4758415461714905E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="7:17">
       <c r="J57" s="16">
         <f>$J$13</f>
         <v>1.5</v>
@@ -3671,14 +3712,15 @@
       <c r="K57" s="16"/>
       <c r="L57" s="18">
         <f>5/(10*J57)-H51/(10*J57*J57)</f>
-        <v>0.19022222222222221</v>
-      </c>
-      <c r="O57">
+        <v>0.20488888888888887</v>
+      </c>
+      <c r="M57" s="9"/>
+      <c r="P57">
         <f>$J$13</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="58" spans="7:16">
+    <row r="58" spans="7:17">
       <c r="J58" s="15">
         <f>$J$14</f>
         <v>2.5</v>
@@ -3686,17 +3728,18 @@
       <c r="K58" s="15"/>
       <c r="L58" s="17">
         <f>8/(10*J58)-H54/(10*J58*J58)</f>
-        <v>0.17280000000000001</v>
-      </c>
-      <c r="O58">
+        <v>0.17808000000000002</v>
+      </c>
+      <c r="M58" s="9"/>
+      <c r="P58">
         <f>$J$14</f>
         <v>2.5</v>
       </c>
     </row>
-    <row r="59" spans="7:16">
+    <row r="59" spans="7:17">
       <c r="L59"/>
     </row>
-    <row r="60" spans="7:16">
+    <row r="60" spans="7:17">
       <c r="G60" t="s">
         <v>7</v>
       </c>
@@ -3712,23 +3755,23 @@
       <c r="L60" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="M60" t="s">
+      <c r="N60" t="s">
         <v>38</v>
       </c>
-      <c r="N60" t="s">
+      <c r="O60" t="s">
         <v>49</v>
       </c>
-      <c r="O60" t="s">
+      <c r="P60" t="s">
         <v>42</v>
       </c>
-      <c r="P60" t="s">
+      <c r="Q60" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="61" spans="7:16">
+    <row r="61" spans="7:17">
       <c r="L61"/>
     </row>
-    <row r="62" spans="7:16">
+    <row r="62" spans="7:17">
       <c r="G62">
         <v>0.3</v>
       </c>
@@ -3749,24 +3792,25 @@
         <f t="shared" ref="L62:L71" si="36">(D3*D3)/($E$3*4*H62)</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="M62">
+      <c r="M62" s="9"/>
+      <c r="N62">
         <f>G62^2</f>
         <v>0.09</v>
       </c>
-      <c r="N62">
-        <f>G62/O62</f>
+      <c r="O62">
+        <f>G62/P62</f>
         <v>0.57735026918962573</v>
       </c>
-      <c r="O62" s="5">
-        <f t="shared" ref="O62:O71" si="37">(3*M62/D3)^(1/2)</f>
+      <c r="P62" s="5">
+        <f t="shared" ref="P62:P71" si="37">(3*N62/D3)^(1/2)</f>
         <v>0.51961524227066325</v>
       </c>
-      <c r="P62" s="5">
-        <f t="shared" ref="P62:P71" si="38">(3/4)*((2*D3^(1/2))/(27^(1/2)*$E$3*M62^(1/2)))</f>
+      <c r="Q62" s="5">
+        <f t="shared" ref="Q62:Q71" si="38">(3/4)*((2*D3^(1/2))/(27^(1/2)*$E$3*N62^(1/2)))</f>
         <v>9.6225044864937617E-2</v>
       </c>
     </row>
-    <row r="63" spans="7:16">
+    <row r="63" spans="7:17">
       <c r="G63">
         <v>0.7</v>
       </c>
@@ -3786,24 +3830,25 @@
         <f t="shared" si="36"/>
         <v>0.1</v>
       </c>
-      <c r="M63">
-        <f t="shared" ref="M63:M71" si="40">M62+G63^2</f>
+      <c r="M63" s="9"/>
+      <c r="N63">
+        <f t="shared" ref="N63:N71" si="40">N62+G63^2</f>
         <v>0.57999999999999996</v>
       </c>
-      <c r="N63">
-        <f t="shared" ref="N63:N71" si="41">G63/O63</f>
+      <c r="O63">
+        <f t="shared" ref="O63:O71" si="41">G63/P63</f>
         <v>0.75047877438645638</v>
       </c>
-      <c r="O63">
+      <c r="P63">
         <f t="shared" si="37"/>
         <v>0.93273790530888145</v>
       </c>
-      <c r="P63">
+      <c r="Q63">
         <f t="shared" si="38"/>
         <v>5.3605626741889748E-2</v>
       </c>
     </row>
-    <row r="64" spans="7:16">
+    <row r="64" spans="7:17">
       <c r="G64">
         <v>0.97</v>
       </c>
@@ -3823,24 +3868,25 @@
         <f t="shared" si="36"/>
         <v>0.11421319796954316</v>
       </c>
-      <c r="M64">
+      <c r="M64" s="9"/>
+      <c r="N64">
         <f t="shared" si="40"/>
         <v>1.5208999999999999</v>
       </c>
-      <c r="N64">
+      <c r="O64">
         <f t="shared" si="41"/>
         <v>0.78654106938960544</v>
       </c>
-      <c r="O64">
+      <c r="P64">
         <f t="shared" si="37"/>
         <v>1.2332477447779906</v>
       </c>
-      <c r="P64">
+      <c r="Q64">
         <f t="shared" si="38"/>
         <v>4.0543354092247706E-2</v>
       </c>
     </row>
-    <row r="65" spans="7:16">
+    <row r="65" spans="7:17">
       <c r="G65">
         <v>1.05</v>
       </c>
@@ -3861,24 +3907,25 @@
         <f t="shared" si="36"/>
         <v>0.13245033112582782</v>
       </c>
-      <c r="M65">
+      <c r="M65" s="9"/>
+      <c r="N65">
         <f t="shared" si="40"/>
         <v>2.6234000000000002</v>
       </c>
-      <c r="N65">
+      <c r="O65">
         <f t="shared" si="41"/>
         <v>0.74855964459154234</v>
       </c>
-      <c r="O65">
+      <c r="P65">
         <f t="shared" si="37"/>
         <v>1.402693836872466</v>
       </c>
-      <c r="P65">
+      <c r="Q65">
         <f t="shared" si="38"/>
         <v>3.5645697361502013E-2</v>
       </c>
     </row>
-    <row r="66" spans="7:16">
+    <row r="66" spans="7:17">
       <c r="G66">
         <v>1.1599999999999999</v>
       </c>
@@ -3898,24 +3945,25 @@
         <f t="shared" si="36"/>
         <v>0.14952153110047847</v>
       </c>
-      <c r="M66">
+      <c r="M66" s="9"/>
+      <c r="N66">
         <f t="shared" si="40"/>
         <v>3.9690000000000003</v>
       </c>
-      <c r="N66">
+      <c r="O66">
         <f t="shared" si="41"/>
         <v>0.75169526498108108</v>
       </c>
-      <c r="O66">
+      <c r="P66">
         <f t="shared" si="37"/>
         <v>1.5431785379534022</v>
       </c>
-      <c r="P66">
+      <c r="Q66">
         <f t="shared" si="38"/>
         <v>3.2400657973322464E-2</v>
       </c>
     </row>
-    <row r="67" spans="7:16">
+    <row r="67" spans="7:17">
       <c r="G67">
         <v>1.31</v>
       </c>
@@ -3935,24 +3983,25 @@
         <f t="shared" si="36"/>
         <v>0.16393442622950818</v>
       </c>
-      <c r="M67">
+      <c r="M67" s="9"/>
+      <c r="N67">
         <f t="shared" si="40"/>
         <v>5.6851000000000003</v>
       </c>
-      <c r="N67">
+      <c r="O67">
         <f t="shared" si="41"/>
         <v>0.77699323819381194</v>
       </c>
-      <c r="O67">
+      <c r="P67">
         <f t="shared" si="37"/>
         <v>1.6859863581891761</v>
       </c>
-      <c r="P67">
+      <c r="Q67">
         <f t="shared" si="38"/>
         <v>2.9656230465412665E-2</v>
       </c>
     </row>
-    <row r="68" spans="7:16">
+    <row r="68" spans="7:17">
       <c r="G68">
         <v>1.38</v>
       </c>
@@ -3972,24 +4021,25 @@
         <f t="shared" si="36"/>
         <v>0.17831149927219794</v>
       </c>
-      <c r="M68">
+      <c r="M68" s="9"/>
+      <c r="N68">
         <f t="shared" si="40"/>
         <v>7.5895000000000001</v>
       </c>
-      <c r="N68">
+      <c r="O68">
         <f t="shared" si="41"/>
         <v>0.76517521881494821</v>
       </c>
-      <c r="O68">
+      <c r="P68">
         <f t="shared" si="37"/>
         <v>1.8035084854646115</v>
       </c>
-      <c r="P68">
+      <c r="Q68">
         <f t="shared" si="38"/>
         <v>2.7723739812135807E-2</v>
       </c>
     </row>
-    <row r="69" spans="7:16">
+    <row r="69" spans="7:17">
       <c r="G69">
         <v>1.7</v>
       </c>
@@ -4009,24 +4059,25 @@
         <f t="shared" si="36"/>
         <v>0.1866977829638273</v>
       </c>
-      <c r="M69">
-        <f t="shared" si="40"/>
+      <c r="M69" s="9"/>
+      <c r="N69">
+        <f>N68+G69^2</f>
         <v>10.4795</v>
       </c>
-      <c r="N69">
-        <f t="shared" si="41"/>
+      <c r="O69">
+        <f>G69/P69</f>
         <v>0.85755702015303192</v>
       </c>
-      <c r="O69">
-        <f t="shared" si="37"/>
+      <c r="P69">
+        <f>(3*N69/D10)^(1/2)</f>
         <v>1.9823754689765507</v>
       </c>
-      <c r="P69">
-        <f t="shared" si="38"/>
+      <c r="Q69">
+        <f>(3/4)*((2*D10^(1/2))/(27^(1/2)*$E$3*N69^(1/2)))</f>
         <v>2.5222265298618589E-2</v>
       </c>
     </row>
-    <row r="70" spans="7:16">
+    <row r="70" spans="7:17">
       <c r="G70">
         <v>2</v>
       </c>
@@ -4047,24 +4098,25 @@
         <f t="shared" si="36"/>
         <v>0.19157994323557237</v>
       </c>
-      <c r="M70">
-        <f t="shared" si="40"/>
+      <c r="M70" s="9"/>
+      <c r="N70">
+        <f>N69+G70^2</f>
         <v>14.4795</v>
       </c>
-      <c r="N70">
+      <c r="O70">
         <f t="shared" si="41"/>
         <v>0.91036141125309444</v>
       </c>
-      <c r="O70" s="11">
+      <c r="P70" s="11">
         <f t="shared" si="37"/>
         <v>2.1969296757065302</v>
       </c>
-      <c r="P70" s="11">
+      <c r="Q70" s="11">
         <f t="shared" si="38"/>
         <v>2.2759035281327361E-2</v>
       </c>
     </row>
-    <row r="71" spans="7:16">
+    <row r="71" spans="7:17">
       <c r="G71">
         <v>3</v>
       </c>
@@ -4085,24 +4137,25 @@
         <f t="shared" si="36"/>
         <v>0.1842299189388357</v>
       </c>
-      <c r="M71">
+      <c r="M71" s="9"/>
+      <c r="N71">
         <f t="shared" si="40"/>
         <v>23.479500000000002</v>
       </c>
-      <c r="N71" s="21">
+      <c r="O71" s="21">
         <f t="shared" si="41"/>
         <v>1.1303585020095293</v>
       </c>
-      <c r="O71" s="21">
+      <c r="P71" s="21">
         <f t="shared" si="37"/>
         <v>2.6540252447932744</v>
       </c>
-      <c r="P71" s="21">
+      <c r="Q71" s="21">
         <f t="shared" si="38"/>
         <v>1.8839308366825486E-2</v>
       </c>
     </row>
-    <row r="72" spans="7:16">
+    <row r="72" spans="7:17">
       <c r="J72">
         <f>$J$13</f>
         <v>1.5</v>
@@ -4111,12 +4164,13 @@
         <f>7/(10*J72)-H68/(10*J72*J72)</f>
         <v>0.16133333333333333</v>
       </c>
-      <c r="O72">
+      <c r="M72" s="9"/>
+      <c r="P72">
         <f>$J$13</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="73" spans="7:16">
+    <row r="73" spans="7:17">
       <c r="J73">
         <f>$J$14</f>
         <v>2.5</v>
@@ -4125,15 +4179,16 @@
         <f>9/(10*J73)-H70/(10*J73*J73)</f>
         <v>0.19087999999999999</v>
       </c>
-      <c r="O73">
+      <c r="M73" s="9"/>
+      <c r="P73">
         <f>$J$14</f>
         <v>2.5</v>
       </c>
     </row>
-    <row r="74" spans="7:16">
+    <row r="74" spans="7:17">
       <c r="L74"/>
     </row>
-    <row r="75" spans="7:16">
+    <row r="75" spans="7:17">
       <c r="G75" t="s">
         <v>8</v>
       </c>
@@ -4149,23 +4204,23 @@
       <c r="L75" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="M75" t="s">
+      <c r="N75" t="s">
         <v>38</v>
       </c>
-      <c r="N75" t="s">
+      <c r="O75" t="s">
         <v>49</v>
       </c>
-      <c r="O75" t="s">
+      <c r="P75" t="s">
         <v>42</v>
       </c>
-      <c r="P75" t="s">
+      <c r="Q75" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="76" spans="7:16">
+    <row r="76" spans="7:17">
       <c r="L76"/>
     </row>
-    <row r="77" spans="7:16">
+    <row r="77" spans="7:17">
       <c r="G77">
         <v>0.03</v>
       </c>
@@ -4186,24 +4241,25 @@
         <f t="shared" ref="L77:L86" si="44">(D3*D3)/($E$3*4*H77)</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="M77">
+      <c r="M77" s="9"/>
+      <c r="N77">
         <f>G77^2</f>
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="N77">
-        <f>G77/O77</f>
+      <c r="O77">
+        <f>G77/P77</f>
         <v>0.57735026918962573</v>
       </c>
-      <c r="O77" s="5">
-        <f t="shared" ref="O77:O86" si="45">(3*M77/D3)^(1/2)</f>
+      <c r="P77" s="5">
+        <f t="shared" ref="P77:P86" si="45">(3*N77/D3)^(1/2)</f>
         <v>5.1961524227066319E-2</v>
       </c>
-      <c r="P77" s="5">
-        <f t="shared" ref="P77:P86" si="46">(3/4)*((2*D3^(1/2))/(27^(1/2)*$E$3*M77^(1/2)))</f>
+      <c r="Q77" s="5">
+        <f t="shared" ref="Q77:Q86" si="46">(3/4)*((2*D3^(1/2))/(27^(1/2)*$E$3*N77^(1/2)))</f>
         <v>0.96225044864937626</v>
       </c>
     </row>
-    <row r="78" spans="7:16">
+    <row r="78" spans="7:17">
       <c r="G78">
         <v>0.3</v>
       </c>
@@ -4223,24 +4279,25 @@
         <f t="shared" si="44"/>
         <v>0.30303030303030304</v>
       </c>
-      <c r="M78">
-        <f t="shared" ref="M78:M86" si="48">M77+G78^2</f>
+      <c r="M78" s="9"/>
+      <c r="N78">
+        <f t="shared" ref="N78:N86" si="48">N77+G78^2</f>
         <v>9.0899999999999995E-2</v>
       </c>
-      <c r="N78">
-        <f t="shared" ref="N78:N86" si="49">G78/O78</f>
+      <c r="O78">
+        <f t="shared" ref="O78:O86" si="49">G78/P78</f>
         <v>0.81244446370238754</v>
       </c>
-      <c r="O78">
+      <c r="P78">
         <f t="shared" si="45"/>
         <v>0.36925600875273512</v>
       </c>
-      <c r="P78">
+      <c r="Q78">
         <f t="shared" si="46"/>
         <v>0.13540741061706457</v>
       </c>
     </row>
-    <row r="79" spans="7:16">
+    <row r="79" spans="7:17">
       <c r="G79">
         <v>0.31</v>
       </c>
@@ -4260,24 +4317,25 @@
         <f t="shared" si="44"/>
         <v>0.35156250000000006</v>
       </c>
-      <c r="M79">
+      <c r="M79" s="9"/>
+      <c r="N79">
         <f t="shared" si="48"/>
         <v>0.187</v>
       </c>
-      <c r="N79">
+      <c r="O79">
         <f t="shared" si="49"/>
         <v>0.71687079959746447</v>
       </c>
-      <c r="O79">
+      <c r="P79">
         <f t="shared" si="45"/>
         <v>0.43243496620879301</v>
       </c>
-      <c r="P79">
+      <c r="Q79">
         <f t="shared" si="46"/>
         <v>0.11562432251572005</v>
       </c>
     </row>
-    <row r="80" spans="7:16">
+    <row r="80" spans="7:17">
       <c r="G80">
         <v>0.7</v>
       </c>
@@ -4298,24 +4356,25 @@
         <f t="shared" si="44"/>
         <v>0.29850746268656719</v>
       </c>
-      <c r="M80">
+      <c r="M80" s="9"/>
+      <c r="N80">
         <f t="shared" si="48"/>
         <v>0.67699999999999994</v>
       </c>
-      <c r="N80">
+      <c r="O80">
         <f t="shared" si="49"/>
         <v>0.98236543674173316</v>
       </c>
-      <c r="O80">
+      <c r="P80">
         <f t="shared" si="45"/>
         <v>0.71256578643659274</v>
       </c>
-      <c r="P80">
+      <c r="Q80">
         <f t="shared" si="46"/>
         <v>7.0168959767266642E-2</v>
       </c>
     </row>
-    <row r="81" spans="7:16">
+    <row r="81" spans="7:17">
       <c r="G81">
         <v>0.7</v>
       </c>
@@ -4335,24 +4394,25 @@
         <f t="shared" si="44"/>
         <v>0.30637254901960786</v>
       </c>
-      <c r="M81">
+      <c r="M81" s="9"/>
+      <c r="N81">
         <f t="shared" si="48"/>
         <v>1.1669999999999998</v>
       </c>
-      <c r="N81">
+      <c r="O81">
         <f t="shared" si="49"/>
         <v>0.83654052927908706</v>
       </c>
-      <c r="O81">
+      <c r="P81">
         <f t="shared" si="45"/>
         <v>0.83677954085888118</v>
       </c>
-      <c r="P81">
+      <c r="Q81">
         <f t="shared" si="46"/>
         <v>5.9752894948506226E-2</v>
       </c>
     </row>
-    <row r="82" spans="7:16">
+    <row r="82" spans="7:17">
       <c r="G82">
         <v>2</v>
       </c>
@@ -4373,24 +4433,25 @@
         <f t="shared" si="44"/>
         <v>0.22277227722772278</v>
       </c>
-      <c r="M82">
+      <c r="M82" s="9"/>
+      <c r="N82">
         <f t="shared" si="48"/>
         <v>5.1669999999999998</v>
       </c>
-      <c r="N82" s="21">
+      <c r="O82" s="21">
         <f t="shared" si="49"/>
         <v>1.2443018955530647</v>
       </c>
-      <c r="O82" s="21">
+      <c r="P82" s="21">
         <f t="shared" si="45"/>
         <v>1.6073269735806712</v>
       </c>
-      <c r="P82" s="21">
+      <c r="Q82" s="21">
         <f t="shared" si="46"/>
         <v>3.1107547388826616E-2</v>
       </c>
     </row>
-    <row r="83" spans="7:16">
+    <row r="83" spans="7:17">
       <c r="G83">
         <v>2.0499999999999998</v>
       </c>
@@ -4411,24 +4472,25 @@
         <f t="shared" si="44"/>
         <v>0.20114942528735633</v>
       </c>
-      <c r="M83">
+      <c r="M83" s="9"/>
+      <c r="N83">
         <f t="shared" si="48"/>
         <v>9.3694999999999986</v>
       </c>
-      <c r="N83" s="21">
+      <c r="O83" s="21">
         <f t="shared" si="49"/>
         <v>1.0230198155562749</v>
       </c>
-      <c r="O83" s="21">
+      <c r="P83" s="21">
         <f t="shared" si="45"/>
         <v>2.0038712533493759</v>
       </c>
-      <c r="P83" s="21">
+      <c r="Q83" s="21">
         <f t="shared" si="46"/>
         <v>2.4951702818445727E-2</v>
       </c>
     </row>
-    <row r="84" spans="7:16">
+    <row r="84" spans="7:17">
       <c r="G84">
         <v>2.16</v>
       </c>
@@ -4449,24 +4511,25 @@
         <f t="shared" si="44"/>
         <v>0.19393939393939394</v>
       </c>
-      <c r="M84">
+      <c r="M84" s="9"/>
+      <c r="N84">
         <f t="shared" si="48"/>
         <v>14.0351</v>
       </c>
-      <c r="N84">
+      <c r="O84">
         <f t="shared" si="49"/>
         <v>0.94152175988910569</v>
       </c>
-      <c r="O84">
+      <c r="P84">
         <f t="shared" si="45"/>
         <v>2.2941583423992338</v>
       </c>
-      <c r="P84">
+      <c r="Q84">
         <f t="shared" si="46"/>
         <v>2.1794485182618187E-2</v>
       </c>
     </row>
-    <row r="85" spans="7:16">
+    <row r="85" spans="7:17">
       <c r="G85">
         <v>2.38</v>
       </c>
@@ -4487,24 +4550,25 @@
         <f t="shared" si="44"/>
         <v>0.19049858889934151</v>
       </c>
-      <c r="M85">
+      <c r="M85" s="9"/>
+      <c r="N85">
         <f t="shared" si="48"/>
         <v>19.6995</v>
       </c>
-      <c r="N85">
+      <c r="O85">
         <f t="shared" si="49"/>
         <v>0.92877385767607878</v>
       </c>
-      <c r="O85" s="11">
+      <c r="P85" s="11">
         <f t="shared" si="45"/>
         <v>2.5625182926176353</v>
       </c>
-      <c r="P85" s="11">
+      <c r="Q85" s="11">
         <f t="shared" si="46"/>
         <v>1.9512055833531071E-2</v>
       </c>
     </row>
-    <row r="86" spans="7:16">
+    <row r="86" spans="7:17">
       <c r="G86">
         <v>3</v>
       </c>
@@ -4525,33 +4589,34 @@
         <f t="shared" si="44"/>
         <v>0.18341892883345565</v>
       </c>
-      <c r="M86">
+      <c r="M86" s="9"/>
+      <c r="N86">
         <f t="shared" si="48"/>
         <v>28.6995</v>
       </c>
-      <c r="N86" s="21">
+      <c r="O86" s="21">
         <f t="shared" si="49"/>
         <v>1.0224061709023833</v>
       </c>
-      <c r="O86" s="21">
+      <c r="P86" s="21">
         <f t="shared" si="45"/>
         <v>2.9342545901812951</v>
       </c>
-      <c r="P86" s="21">
+      <c r="Q86" s="21">
         <f t="shared" si="46"/>
         <v>1.7040102848373054E-2</v>
       </c>
     </row>
-    <row r="87" spans="7:16">
+    <row r="87" spans="7:17">
       <c r="L87" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="O87">
+      <c r="P87">
         <f>$J$13</f>
         <v>1.5</v>
       </c>
     </row>
-    <row r="88" spans="7:16">
+    <row r="88" spans="7:17">
       <c r="J88" s="19">
         <v>1.5</v>
       </c>
@@ -4560,12 +4625,13 @@
         <f>5/(10*J88)-H81/(10*J88*J88)</f>
         <v>0.24266666666666664</v>
       </c>
-      <c r="O88">
+      <c r="M88" s="9"/>
+      <c r="P88">
         <f>$J$14</f>
         <v>2.5</v>
       </c>
     </row>
-    <row r="89" spans="7:16">
+    <row r="89" spans="7:17">
       <c r="J89" s="20">
         <v>2.5</v>
       </c>
@@ -4575,10 +4641,10 @@
         <v>0.18992000000000001</v>
       </c>
     </row>
-    <row r="90" spans="7:16">
+    <row r="90" spans="7:17">
       <c r="L90"/>
     </row>
-    <row r="91" spans="7:16">
+    <row r="91" spans="7:17">
       <c r="G91" t="s">
         <v>9</v>
       </c>
@@ -4594,23 +4660,23 @@
       <c r="L91" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="M91" t="s">
+      <c r="N91" t="s">
         <v>38</v>
       </c>
-      <c r="N91" t="s">
+      <c r="O91" t="s">
         <v>49</v>
       </c>
-      <c r="O91" t="s">
+      <c r="P91" t="s">
         <v>42</v>
       </c>
-      <c r="P91" t="s">
+      <c r="Q91" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="92" spans="7:16">
+    <row r="92" spans="7:17">
       <c r="L92"/>
     </row>
-    <row r="93" spans="7:16">
+    <row r="93" spans="7:17">
       <c r="G93">
         <v>0.3</v>
       </c>
@@ -4631,24 +4697,25 @@
         <f t="shared" ref="L93:L102" si="52">(D3*D3)/($E$3*4*H93)</f>
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="M93">
+      <c r="M93" s="9"/>
+      <c r="N93">
         <f>G93^2</f>
         <v>0.09</v>
       </c>
-      <c r="N93">
-        <f>G93/O93</f>
+      <c r="O93">
+        <f>G93/P93</f>
         <v>0.57735026918962573</v>
       </c>
-      <c r="O93" s="5">
-        <f t="shared" ref="O93:O102" si="53">(3*M93/D3)^(1/2)</f>
+      <c r="P93" s="5">
+        <f t="shared" ref="P93:P102" si="53">(3*N93/D3)^(1/2)</f>
         <v>0.51961524227066325</v>
       </c>
-      <c r="P93" s="5">
-        <f t="shared" ref="P93:P102" si="54">(3/4)*((2*D3^(1/2))/(27^(1/2)*$E$3*M93^(1/2)))</f>
+      <c r="Q93" s="5">
+        <f t="shared" ref="Q93:Q102" si="54">(3/4)*((2*D3^(1/2))/(27^(1/2)*$E$3*N93^(1/2)))</f>
         <v>9.6225044864937617E-2</v>
       </c>
     </row>
-    <row r="94" spans="7:16">
+    <row r="94" spans="7:17">
       <c r="G94">
         <v>0.69</v>
       </c>
@@ -4668,24 +4735,25 @@
         <f t="shared" si="52"/>
         <v>0.10101010101010101</v>
       </c>
-      <c r="M94">
-        <f t="shared" ref="M94:M102" si="56">M93+G94^2</f>
+      <c r="M94" s="9"/>
+      <c r="N94">
+        <f t="shared" ref="N94:N102" si="56">N93+G94^2</f>
         <v>0.56609999999999994</v>
       </c>
-      <c r="N94">
-        <f t="shared" ref="N94:N102" si="57">G94/O94</f>
+      <c r="O94">
+        <f t="shared" ref="O94:O102" si="57">G94/P94</f>
         <v>0.7487845654019637</v>
       </c>
-      <c r="O94">
+      <c r="P94">
         <f t="shared" si="53"/>
         <v>0.92149335320446013</v>
       </c>
-      <c r="P94">
+      <c r="Q94">
         <f t="shared" si="54"/>
         <v>5.4259751116084338E-2</v>
       </c>
     </row>
-    <row r="95" spans="7:16">
+    <row r="95" spans="7:17">
       <c r="G95">
         <v>1</v>
       </c>
@@ -4705,24 +4773,25 @@
         <f t="shared" si="52"/>
         <v>0.11306532663316583</v>
       </c>
-      <c r="M95">
+      <c r="M95" s="9"/>
+      <c r="N95">
         <f t="shared" si="56"/>
         <v>1.5661</v>
       </c>
-      <c r="N95">
+      <c r="O95">
         <f t="shared" si="57"/>
         <v>0.79907998947330394</v>
       </c>
-      <c r="O95">
+      <c r="P95">
         <f t="shared" si="53"/>
         <v>1.2514391715141411</v>
       </c>
-      <c r="P95">
+      <c r="Q95">
         <f t="shared" si="54"/>
         <v>3.9953999473665187E-2</v>
       </c>
     </row>
-    <row r="96" spans="7:16">
+    <row r="96" spans="7:17">
       <c r="G96">
         <v>1.03</v>
       </c>
@@ -4743,24 +4812,25 @@
         <f t="shared" si="52"/>
         <v>0.13245033112582782</v>
       </c>
-      <c r="M96">
+      <c r="M96" s="9"/>
+      <c r="N96">
         <f t="shared" si="56"/>
         <v>2.6269999999999998</v>
       </c>
-      <c r="N96">
+      <c r="O96">
         <f t="shared" si="57"/>
         <v>0.73379805556223054</v>
       </c>
-      <c r="O96">
+      <c r="P96">
         <f t="shared" si="53"/>
         <v>1.4036559407490141</v>
       </c>
-      <c r="P96">
+      <c r="Q96">
         <f t="shared" si="54"/>
         <v>3.5621264833117977E-2</v>
       </c>
     </row>
-    <row r="97" spans="7:16">
+    <row r="97" spans="7:17">
       <c r="G97">
         <v>1.3</v>
       </c>
@@ -4780,24 +4850,25 @@
         <f t="shared" si="52"/>
         <v>0.14467592592592593</v>
       </c>
-      <c r="M97">
+      <c r="M97" s="9"/>
+      <c r="N97">
         <f t="shared" si="56"/>
         <v>4.3170000000000002</v>
       </c>
-      <c r="N97">
+      <c r="O97">
         <f t="shared" si="57"/>
         <v>0.807749509163871</v>
       </c>
-      <c r="O97">
+      <c r="P97">
         <f t="shared" si="53"/>
         <v>1.6094098297201991</v>
       </c>
-      <c r="P97">
+      <c r="Q97">
         <f t="shared" si="54"/>
         <v>3.106728881399504E-2</v>
       </c>
     </row>
-    <row r="98" spans="7:16">
+    <row r="98" spans="7:17">
       <c r="G98">
         <v>1.7</v>
       </c>
@@ -4818,24 +4889,25 @@
         <f t="shared" si="52"/>
         <v>0.14950166112956809</v>
       </c>
-      <c r="M98">
+      <c r="M98" s="9"/>
+      <c r="N98">
         <f t="shared" si="56"/>
         <v>7.2069999999999999</v>
       </c>
-      <c r="N98">
+      <c r="O98">
         <f t="shared" si="57"/>
         <v>0.89554344252199825</v>
       </c>
-      <c r="O98">
+      <c r="P98">
         <f t="shared" si="53"/>
         <v>1.8982887030164826</v>
       </c>
-      <c r="P98">
+      <c r="Q98">
         <f t="shared" si="54"/>
         <v>2.6339513015352888E-2</v>
       </c>
     </row>
-    <row r="99" spans="7:16">
+    <row r="99" spans="7:17">
       <c r="G99">
         <v>3.05</v>
       </c>
@@ -4856,24 +4928,25 @@
         <f t="shared" si="52"/>
         <v>0.13506063947078278</v>
       </c>
-      <c r="M99">
+      <c r="M99" s="9"/>
+      <c r="N99">
         <f t="shared" si="56"/>
         <v>16.509499999999999</v>
       </c>
-      <c r="N99" s="21">
+      <c r="O99" s="21">
         <f t="shared" si="57"/>
         <v>1.1466246440492356</v>
       </c>
-      <c r="O99" s="21">
+      <c r="P99" s="21">
         <f t="shared" si="53"/>
         <v>2.6599812029411032</v>
       </c>
-      <c r="P99" s="21">
+      <c r="Q99" s="21">
         <f t="shared" si="54"/>
         <v>1.8797125312282552E-2</v>
       </c>
     </row>
-    <row r="100" spans="7:16">
+    <row r="100" spans="7:17">
       <c r="G100">
         <v>3.16</v>
       </c>
@@ -4894,24 +4967,25 @@
         <f t="shared" si="52"/>
         <v>0.13082583810302534</v>
       </c>
-      <c r="M100">
+      <c r="M100" s="9"/>
+      <c r="N100">
         <f t="shared" si="56"/>
         <v>26.495100000000001</v>
       </c>
-      <c r="N100" s="21">
+      <c r="O100" s="21">
         <f t="shared" si="57"/>
         <v>1.0025098935095671</v>
       </c>
-      <c r="O100" s="21">
+      <c r="P100" s="21">
         <f t="shared" si="53"/>
         <v>3.1520885932981009</v>
       </c>
-      <c r="P100" s="21">
+      <c r="Q100" s="21">
         <f t="shared" si="54"/>
         <v>1.5862498315024794E-2</v>
       </c>
     </row>
-    <row r="101" spans="7:16">
+    <row r="101" spans="7:17">
       <c r="G101">
         <v>3.38</v>
       </c>
@@ -4932,24 +5006,25 @@
         <f t="shared" si="52"/>
         <v>0.12972453555413196</v>
       </c>
-      <c r="M101">
+      <c r="M101" s="9"/>
+      <c r="N101">
         <f t="shared" si="56"/>
         <v>37.919499999999999</v>
       </c>
-      <c r="N101">
+      <c r="O101">
         <f t="shared" si="57"/>
         <v>0.95070554414033615</v>
       </c>
-      <c r="O101">
+      <c r="P101">
         <f t="shared" si="53"/>
         <v>3.5552543275177002</v>
       </c>
-      <c r="P101">
+      <c r="Q101">
         <f t="shared" si="54"/>
         <v>1.4063691481365921E-2</v>
       </c>
     </row>
-    <row r="102" spans="7:16">
+    <row r="102" spans="7:17">
       <c r="G102">
         <v>4</v>
       </c>
@@ -4970,24 +5045,25 @@
         <f t="shared" si="52"/>
         <v>0.12748597654258031</v>
       </c>
-      <c r="M102">
+      <c r="M102" s="9"/>
+      <c r="N102">
         <f t="shared" si="56"/>
         <v>53.919499999999999</v>
       </c>
-      <c r="N102">
+      <c r="O102">
         <f t="shared" si="57"/>
         <v>0.99454957426497603</v>
       </c>
-      <c r="O102" s="11">
+      <c r="P102" s="11">
         <f t="shared" si="53"/>
         <v>4.0219211827185273</v>
       </c>
-      <c r="P102" s="11">
+      <c r="Q102" s="11">
         <f t="shared" si="54"/>
         <v>1.24318696783122E-2</v>
       </c>
     </row>
-    <row r="103" spans="7:16">
+    <row r="103" spans="7:17">
       <c r="J103" s="1">
         <v>1.5</v>
       </c>
@@ -4996,11 +5072,12 @@
         <f>5/(10*J103)-H97/(10*J103*J103)</f>
         <v>0.14133333333333331</v>
       </c>
-      <c r="O103" s="1">
+      <c r="M103" s="9"/>
+      <c r="P103" s="1">
         <v>1.5</v>
       </c>
     </row>
-    <row r="104" spans="7:16">
+    <row r="104" spans="7:17">
       <c r="J104" s="1">
         <v>2.5</v>
       </c>
@@ -5009,14 +5086,15 @@
         <f>6/(10*J104)-H98/(10*J104*J104)</f>
         <v>0.14367999999999997</v>
       </c>
-      <c r="O104" s="1">
+      <c r="M104" s="9"/>
+      <c r="P104" s="1">
         <v>2.5</v>
       </c>
     </row>
-    <row r="105" spans="7:16">
+    <row r="105" spans="7:17">
       <c r="L105"/>
     </row>
-    <row r="106" spans="7:16">
+    <row r="106" spans="7:17">
       <c r="G106" t="s">
         <v>10</v>
       </c>
@@ -5032,23 +5110,23 @@
       <c r="L106" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="M106" t="s">
+      <c r="N106" t="s">
         <v>38</v>
       </c>
-      <c r="N106" t="s">
+      <c r="O106" t="s">
         <v>49</v>
       </c>
-      <c r="O106" t="s">
+      <c r="P106" t="s">
         <v>42</v>
       </c>
-      <c r="P106" t="s">
+      <c r="Q106" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="107" spans="7:16">
+    <row r="107" spans="7:17">
       <c r="L107"/>
     </row>
-    <row r="108" spans="7:16">
+    <row r="108" spans="7:17">
       <c r="G108">
         <v>0</v>
       </c>
@@ -5068,24 +5146,25 @@
         <f t="shared" ref="L108:L117" si="60">(D3*D3)/($E$3*4*H108)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M108">
+      <c r="M108" s="9"/>
+      <c r="N108">
         <f>G108^2</f>
         <v>0</v>
       </c>
-      <c r="N108" t="e">
-        <f>G108/O108</f>
+      <c r="O108" t="e">
+        <f>G108/P108</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="O108">
-        <f t="shared" ref="O108:O117" si="61">(3*M108/D3)^(1/2)</f>
+      <c r="P108">
+        <f t="shared" ref="P108:P117" si="61">(3*N108/D3)^(1/2)</f>
         <v>0</v>
       </c>
-      <c r="P108" t="e">
-        <f t="shared" ref="P108:P117" si="62">(3/4)*((2*D3^(1/2))/(27^(1/2)*$E$3*M108^(1/2)))</f>
+      <c r="Q108" t="e">
+        <f t="shared" ref="Q108:Q117" si="62">(3/4)*((2*D3^(1/2))/(27^(1/2)*$E$3*N108^(1/2)))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="109" spans="7:16">
+    <row r="109" spans="7:17">
       <c r="G109">
         <v>1.3</v>
       </c>
@@ -5105,24 +5184,25 @@
         <f t="shared" si="60"/>
         <v>7.6923076923076927E-2</v>
       </c>
-      <c r="M109">
-        <f t="shared" ref="M109:M117" si="64">M108+G109^2</f>
+      <c r="M109" s="9"/>
+      <c r="N109">
+        <f t="shared" ref="N109:N117" si="64">N108+G109^2</f>
         <v>1.6900000000000002</v>
       </c>
-      <c r="N109">
-        <f t="shared" ref="N109:N117" si="65">G109/O109</f>
+      <c r="O109">
+        <f t="shared" ref="O109:O117" si="65">G109/P109</f>
         <v>0.81649658092772603</v>
       </c>
-      <c r="O109" s="5">
+      <c r="P109" s="5">
         <f t="shared" si="61"/>
         <v>1.5921683328090659</v>
       </c>
-      <c r="P109" s="5">
+      <c r="Q109" s="5">
         <f t="shared" si="62"/>
         <v>3.1403714651066388E-2</v>
       </c>
     </row>
-    <row r="110" spans="7:16">
+    <row r="110" spans="7:17">
       <c r="G110">
         <v>1.69</v>
       </c>
@@ -5143,24 +5223,25 @@
         <f t="shared" si="60"/>
         <v>7.5250836120401329E-2</v>
       </c>
-      <c r="M110">
+      <c r="M110" s="9"/>
+      <c r="N110">
         <f t="shared" si="64"/>
         <v>4.5461</v>
       </c>
-      <c r="N110">
+      <c r="O110">
         <f t="shared" si="65"/>
         <v>0.79262398910460008</v>
       </c>
-      <c r="O110">
+      <c r="P110">
         <f t="shared" si="61"/>
         <v>2.1321585306913744</v>
       </c>
-      <c r="P110">
+      <c r="Q110">
         <f t="shared" si="62"/>
         <v>2.3450413878834318E-2</v>
       </c>
     </row>
-    <row r="111" spans="7:16">
+    <row r="111" spans="7:17">
       <c r="G111">
         <v>2.0299999999999998</v>
       </c>
@@ -5180,24 +5261,25 @@
         <f t="shared" si="60"/>
         <v>7.9681274900398419E-2</v>
       </c>
-      <c r="M111">
+      <c r="M111" s="9"/>
+      <c r="N111">
         <f t="shared" si="64"/>
         <v>8.666999999999998</v>
       </c>
-      <c r="N111">
+      <c r="O111">
         <f t="shared" si="65"/>
         <v>0.79621619695831214</v>
       </c>
-      <c r="O111">
+      <c r="P111">
         <f t="shared" si="61"/>
         <v>2.5495587853587529</v>
       </c>
-      <c r="P111">
+      <c r="Q111">
         <f t="shared" si="62"/>
         <v>1.9611236378283551E-2</v>
       </c>
     </row>
-    <row r="112" spans="7:16">
+    <row r="112" spans="7:17">
       <c r="G112">
         <v>2.2999999999999998</v>
       </c>
@@ -5217,24 +5299,25 @@
         <f t="shared" si="60"/>
         <v>8.5382513661202197E-2</v>
       </c>
-      <c r="M112">
+      <c r="M112" s="9"/>
+      <c r="N112">
         <f t="shared" si="64"/>
         <v>13.956999999999997</v>
       </c>
-      <c r="N112">
+      <c r="O112">
         <f t="shared" si="65"/>
         <v>0.79479691289098375</v>
       </c>
-      <c r="O112">
+      <c r="P112">
         <f t="shared" si="61"/>
         <v>2.8938210034485543</v>
       </c>
-      <c r="P112">
+      <c r="Q112">
         <f t="shared" si="62"/>
         <v>1.7278193758499649E-2</v>
       </c>
     </row>
-    <row r="113" spans="7:16">
+    <row r="113" spans="7:17">
       <c r="G113">
         <v>2.7</v>
       </c>
@@ -5255,24 +5338,25 @@
         <f t="shared" si="60"/>
         <v>8.982035928143714E-2</v>
       </c>
-      <c r="M113">
+      <c r="M113" s="9"/>
+      <c r="N113">
         <f t="shared" si="64"/>
         <v>21.247</v>
       </c>
-      <c r="N113">
+      <c r="O113">
         <f t="shared" si="65"/>
         <v>0.82838066394831145</v>
       </c>
-      <c r="O113">
+      <c r="P113">
         <f t="shared" si="61"/>
         <v>3.2593711049832912</v>
       </c>
-      <c r="P113">
+      <c r="Q113">
         <f t="shared" si="62"/>
         <v>1.534038266570947E-2</v>
       </c>
     </row>
-    <row r="114" spans="7:16">
+    <row r="114" spans="7:17">
       <c r="G114">
         <v>4.05</v>
       </c>
@@ -5293,24 +5377,25 @@
         <f t="shared" si="60"/>
         <v>8.7064676616915429E-2</v>
       </c>
-      <c r="M114">
+      <c r="M114" s="9"/>
+      <c r="N114">
         <f t="shared" si="64"/>
         <v>37.649500000000003</v>
       </c>
-      <c r="N114" s="21">
+      <c r="O114" s="21">
         <f t="shared" si="65"/>
         <v>1.0082397356317756</v>
       </c>
-      <c r="O114" s="21">
+      <c r="P114" s="21">
         <f t="shared" si="61"/>
         <v>4.0169017911818559</v>
       </c>
-      <c r="P114" s="21">
+      <c r="Q114" s="21">
         <f t="shared" si="62"/>
         <v>1.2447404143602167E-2</v>
       </c>
     </row>
-    <row r="115" spans="7:16">
+    <row r="115" spans="7:17">
       <c r="G115">
         <v>4.16</v>
       </c>
@@ -5330,24 +5415,25 @@
         <f t="shared" si="60"/>
         <v>8.7767416346681296E-2</v>
       </c>
-      <c r="M115">
+      <c r="M115" s="9"/>
+      <c r="N115">
         <f t="shared" si="64"/>
         <v>54.955100000000002</v>
       </c>
-      <c r="N115">
+      <c r="O115">
         <f t="shared" si="65"/>
         <v>0.91637597696852457</v>
       </c>
-      <c r="O115">
+      <c r="P115">
         <f t="shared" si="61"/>
         <v>4.5396214049191368</v>
       </c>
-      <c r="P115">
+      <c r="Q115">
         <f t="shared" si="62"/>
         <v>1.1014134338563995E-2</v>
       </c>
     </row>
-    <row r="116" spans="7:16">
+    <row r="116" spans="7:17">
       <c r="G116">
         <v>4.38</v>
       </c>
@@ -5367,24 +5453,25 @@
         <f t="shared" si="60"/>
         <v>8.956214064573198E-2</v>
       </c>
-      <c r="M116">
+      <c r="M116" s="9"/>
+      <c r="N116">
         <f t="shared" si="64"/>
         <v>74.139499999999998</v>
       </c>
-      <c r="N116">
+      <c r="O116">
         <f t="shared" si="65"/>
         <v>0.88106898052257587</v>
       </c>
-      <c r="O116">
+      <c r="P116">
         <f t="shared" si="61"/>
         <v>4.9712339179188367</v>
       </c>
-      <c r="P116">
+      <c r="Q116">
         <f t="shared" si="62"/>
         <v>1.0057865074458629E-2</v>
       </c>
     </row>
-    <row r="117" spans="7:16">
+    <row r="117" spans="7:17">
       <c r="G117">
         <v>5</v>
       </c>
@@ -5405,24 +5492,25 @@
         <f t="shared" si="60"/>
         <v>9.0546903295907269E-2</v>
       </c>
-      <c r="M117">
+      <c r="M117" s="9"/>
+      <c r="N117">
         <f t="shared" si="64"/>
         <v>99.139499999999998</v>
       </c>
-      <c r="N117">
+      <c r="O117">
         <f t="shared" si="65"/>
         <v>0.91682408741692289</v>
       </c>
-      <c r="O117" s="11">
+      <c r="P117" s="11">
         <f t="shared" si="61"/>
         <v>5.4536088968682011</v>
       </c>
-      <c r="P117" s="11">
+      <c r="Q117" s="11">
         <f t="shared" si="62"/>
         <v>9.1682408741692277E-3</v>
       </c>
     </row>
-    <row r="118" spans="7:16">
+    <row r="118" spans="7:17">
       <c r="J118" s="1">
         <v>1.5</v>
       </c>
@@ -5431,11 +5519,12 @@
         <f>2/(10*J118)-H109/(10*J118*J118)</f>
         <v>7.5555555555555542E-2</v>
       </c>
-      <c r="O118" s="1">
+      <c r="M118" s="9"/>
+      <c r="P118" s="1">
         <v>1.5</v>
       </c>
     </row>
-    <row r="119" spans="7:16">
+    <row r="119" spans="7:17">
       <c r="J119" s="19">
         <v>2.5</v>
       </c>
@@ -5444,14 +5533,15 @@
         <f>5/(10*J119)-H112/(10*J119*J119)</f>
         <v>8.2880000000000023E-2</v>
       </c>
-      <c r="O119" s="1">
+      <c r="M119" s="9"/>
+      <c r="P119" s="1">
         <v>2.5</v>
       </c>
     </row>
-    <row r="120" spans="7:16">
+    <row r="120" spans="7:17">
       <c r="L120"/>
     </row>
-    <row r="121" spans="7:16">
+    <row r="121" spans="7:17">
       <c r="G121" t="s">
         <v>11</v>
       </c>
@@ -5467,23 +5557,23 @@
       <c r="L121" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="M121" t="s">
+      <c r="N121" t="s">
         <v>38</v>
       </c>
-      <c r="N121" t="s">
+      <c r="O121" t="s">
         <v>49</v>
       </c>
-      <c r="O121" t="s">
+      <c r="P121" t="s">
         <v>42</v>
       </c>
-      <c r="P121" t="s">
+      <c r="Q121" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="122" spans="7:16">
+    <row r="122" spans="7:17">
       <c r="L122"/>
     </row>
-    <row r="123" spans="7:16">
+    <row r="123" spans="7:17">
       <c r="G123">
         <v>1</v>
       </c>
@@ -5504,24 +5594,25 @@
         <f t="shared" ref="L123:L132" si="68">(D3*D3)/($E$3*4*H123)</f>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="M123">
+      <c r="M123" s="9"/>
+      <c r="N123">
         <f>G123^2</f>
         <v>1</v>
       </c>
-      <c r="N123">
-        <f>G123/O123</f>
+      <c r="O123">
+        <f>G123/P123</f>
         <v>0.57735026918962584</v>
       </c>
-      <c r="O123" s="5">
-        <f t="shared" ref="O123:O132" si="69">(3*M123/D3)^(1/2)</f>
+      <c r="P123" s="5">
+        <f t="shared" ref="P123:P132" si="69">(3*N123/D3)^(1/2)</f>
         <v>1.7320508075688772</v>
       </c>
-      <c r="P123" s="5">
-        <f t="shared" ref="P123:P132" si="70">(3/4)*((2*D3^(1/2))/(27^(1/2)*$E$3*M123^(1/2)))</f>
+      <c r="Q123" s="5">
+        <f t="shared" ref="Q123:Q132" si="70">(3/4)*((2*D3^(1/2))/(27^(1/2)*$E$3*N123^(1/2)))</f>
         <v>2.8867513459481287E-2</v>
       </c>
     </row>
-    <row r="124" spans="7:16">
+    <row r="124" spans="7:17">
       <c r="G124">
         <v>2.2999999999999998</v>
       </c>
@@ -5541,24 +5632,25 @@
         <f t="shared" si="68"/>
         <v>3.0303030303030304E-2</v>
       </c>
-      <c r="M124">
-        <f t="shared" ref="M124:M132" si="72">M123+G124^2</f>
+      <c r="M124" s="9"/>
+      <c r="N124">
+        <f t="shared" ref="N124:N132" si="72">N123+G124^2</f>
         <v>6.2899999999999991</v>
       </c>
-      <c r="N124">
-        <f t="shared" ref="N124:N132" si="73">G124/O124</f>
+      <c r="O124">
+        <f t="shared" ref="O124:O132" si="73">G124/P124</f>
         <v>0.74878456540196381</v>
       </c>
-      <c r="O124">
+      <c r="P124">
         <f t="shared" si="69"/>
         <v>3.0716445106815335</v>
       </c>
-      <c r="P124">
+      <c r="Q124">
         <f t="shared" si="70"/>
         <v>1.6277925334825298E-2</v>
       </c>
     </row>
-    <row r="125" spans="7:16">
+    <row r="125" spans="7:17">
       <c r="G125">
         <v>2.69</v>
       </c>
@@ -5578,24 +5670,25 @@
         <f t="shared" si="68"/>
         <v>3.7562604340567608E-2</v>
       </c>
-      <c r="M125">
+      <c r="M125" s="9"/>
+      <c r="N125">
         <f t="shared" si="72"/>
         <v>13.5261</v>
       </c>
-      <c r="N125">
+      <c r="O125">
         <f t="shared" si="73"/>
         <v>0.7314185710182749</v>
       </c>
-      <c r="O125">
+      <c r="P125">
         <f t="shared" si="69"/>
         <v>3.6777846592752002</v>
       </c>
-      <c r="P125">
+      <c r="Q125">
         <f t="shared" si="70"/>
         <v>1.3595140725246743E-2</v>
       </c>
     </row>
-    <row r="126" spans="7:16">
+    <row r="126" spans="7:17">
       <c r="G126">
         <v>3.03</v>
       </c>
@@ -5615,24 +5708,25 @@
         <f t="shared" si="68"/>
         <v>4.4345898004434593E-2</v>
       </c>
-      <c r="M126">
+      <c r="M126" s="9"/>
+      <c r="N126">
         <f t="shared" si="72"/>
         <v>22.707000000000001</v>
       </c>
-      <c r="N126">
+      <c r="O126">
         <f t="shared" si="73"/>
         <v>0.73422998546438223</v>
       </c>
-      <c r="O126">
+      <c r="P126">
         <f t="shared" si="69"/>
         <v>4.1267723465197355</v>
       </c>
-      <c r="P126">
+      <c r="Q126">
         <f t="shared" si="70"/>
         <v>1.2116006360798386E-2</v>
       </c>
     </row>
-    <row r="127" spans="7:16">
+    <row r="127" spans="7:17">
       <c r="G127">
         <v>3.3</v>
       </c>
@@ -5652,24 +5746,25 @@
         <f t="shared" si="68"/>
         <v>5.073051948051948E-2</v>
       </c>
-      <c r="M127">
+      <c r="M127" s="9"/>
+      <c r="N127">
         <f t="shared" si="72"/>
         <v>33.597000000000001</v>
       </c>
-      <c r="N127">
+      <c r="O127">
         <f t="shared" si="73"/>
         <v>0.73500122854646865</v>
       </c>
-      <c r="O127">
+      <c r="P127">
         <f t="shared" si="69"/>
         <v>4.4897884137228559</v>
       </c>
-      <c r="P127">
+      <c r="Q127">
         <f t="shared" si="70"/>
         <v>1.1136382250704072E-2</v>
       </c>
     </row>
-    <row r="128" spans="7:16">
+    <row r="128" spans="7:17">
       <c r="G128">
         <v>3.7</v>
       </c>
@@ -5689,24 +5784,25 @@
         <f t="shared" si="68"/>
         <v>5.6179775280898882E-2</v>
       </c>
-      <c r="M128">
+      <c r="M128" s="9"/>
+      <c r="N128">
         <f t="shared" si="72"/>
         <v>47.287000000000006</v>
       </c>
-      <c r="N128">
+      <c r="O128">
         <f t="shared" si="73"/>
         <v>0.7609319870727288</v>
       </c>
-      <c r="O128">
+      <c r="P128">
         <f t="shared" si="69"/>
         <v>4.8624582260416389</v>
       </c>
-      <c r="P128">
+      <c r="Q128">
         <f t="shared" si="70"/>
         <v>1.0282864690172007E-2</v>
       </c>
     </row>
-    <row r="129" spans="7:16">
+    <row r="129" spans="7:17">
       <c r="G129">
         <v>5.05</v>
       </c>
@@ -5726,24 +5822,25 @@
         <f t="shared" si="68"/>
         <v>5.8139534883720936E-2</v>
       </c>
-      <c r="M129">
+      <c r="M129" s="9"/>
+      <c r="N129">
         <f t="shared" si="72"/>
         <v>72.789500000000004</v>
       </c>
-      <c r="N129">
+      <c r="O129">
         <f t="shared" si="73"/>
         <v>0.90416023468913287</v>
       </c>
-      <c r="O129">
+      <c r="P129">
         <f t="shared" si="69"/>
         <v>5.5852931883653163</v>
       </c>
-      <c r="P129">
+      <c r="Q129">
         <f t="shared" si="70"/>
         <v>8.9520815315755741E-3</v>
       </c>
     </row>
-    <row r="130" spans="7:16">
+    <row r="130" spans="7:17">
       <c r="G130">
         <v>5.16</v>
       </c>
@@ -5763,24 +5860,25 @@
         <f t="shared" si="68"/>
         <v>6.0998856271444905E-2</v>
       </c>
-      <c r="M130">
+      <c r="M130" s="9"/>
+      <c r="N130">
         <f t="shared" si="72"/>
         <v>99.41510000000001</v>
       </c>
-      <c r="N130">
+      <c r="O130">
         <f t="shared" si="73"/>
         <v>0.84509958981733824</v>
       </c>
-      <c r="O130">
+      <c r="P130">
         <f t="shared" si="69"/>
         <v>6.1057892610210525</v>
       </c>
-      <c r="P130">
+      <c r="Q130">
         <f t="shared" si="70"/>
         <v>8.1889495137338966E-3</v>
       </c>
     </row>
-    <row r="131" spans="7:16">
+    <row r="131" spans="7:17">
       <c r="G131">
         <v>5.38</v>
       </c>
@@ -5800,24 +5898,25 @@
         <f t="shared" si="68"/>
         <v>6.4062005694400501E-2</v>
       </c>
-      <c r="M131">
+      <c r="M131" s="9"/>
+      <c r="N131">
         <f t="shared" si="72"/>
         <v>128.3595</v>
       </c>
-      <c r="N131">
+      <c r="O131">
         <f t="shared" si="73"/>
         <v>0.82248672033521952</v>
       </c>
-      <c r="O131">
+      <c r="P131">
         <f t="shared" si="69"/>
         <v>6.541139044539567</v>
       </c>
-      <c r="P131">
+      <c r="Q131">
         <f t="shared" si="70"/>
         <v>7.6439286276507399E-3</v>
       </c>
     </row>
-    <row r="132" spans="7:16">
+    <row r="132" spans="7:17">
       <c r="G132">
         <v>6</v>
       </c>
@@ -5838,24 +5937,25 @@
         <f t="shared" si="68"/>
         <v>6.6471683063015152E-2</v>
       </c>
-      <c r="M132">
+      <c r="M132" s="9"/>
+      <c r="N132">
         <f t="shared" si="72"/>
         <v>164.3595</v>
       </c>
-      <c r="N132">
+      <c r="O132">
         <f t="shared" si="73"/>
         <v>0.85446291282477993</v>
       </c>
-      <c r="O132" s="11">
+      <c r="P132" s="11">
         <f t="shared" si="69"/>
         <v>7.0219548560212202</v>
       </c>
-      <c r="P132" s="11">
+      <c r="Q132" s="11">
         <f t="shared" si="70"/>
         <v>7.1205242735398327E-3</v>
       </c>
     </row>
-    <row r="133" spans="7:16">
+    <row r="133" spans="7:17">
       <c r="J133" s="20">
         <v>1.5</v>
       </c>
@@ -5864,11 +5964,12 @@
         <f>1/(10*J133)-H123/(10*J133*J133)</f>
         <v>2.222222222222222E-2</v>
       </c>
-      <c r="O133" s="1">
+      <c r="M133" s="9"/>
+      <c r="P133" s="1">
         <v>1.5</v>
       </c>
     </row>
-    <row r="134" spans="7:16">
+    <row r="134" spans="7:17">
       <c r="J134" s="19">
         <v>2.5</v>
       </c>
@@ -5877,14 +5978,15 @@
         <f>2/(10*J134)-H124/(10*J134*J134)</f>
         <v>2.7200000000000002E-2</v>
       </c>
-      <c r="O134" s="1">
+      <c r="M134" s="9"/>
+      <c r="P134" s="1">
         <v>2.5</v>
       </c>
     </row>
-    <row r="135" spans="7:16">
+    <row r="135" spans="7:17">
       <c r="L135"/>
     </row>
-    <row r="136" spans="7:16">
+    <row r="136" spans="7:17">
       <c r="G136" t="s">
         <v>12</v>
       </c>
@@ -5900,23 +6002,23 @@
       <c r="L136" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="M136" t="s">
+      <c r="N136" t="s">
         <v>38</v>
       </c>
-      <c r="N136" t="s">
+      <c r="O136" t="s">
         <v>49</v>
       </c>
-      <c r="O136" t="s">
+      <c r="P136" t="s">
         <v>42</v>
       </c>
-      <c r="P136" t="s">
+      <c r="Q136" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="137" spans="7:16">
+    <row r="137" spans="7:17">
       <c r="L137"/>
     </row>
-    <row r="138" spans="7:16">
+    <row r="138" spans="7:17">
       <c r="G138">
         <v>2</v>
       </c>
@@ -5937,24 +6039,25 @@
         <f t="shared" ref="L138:L147" si="76">(D3*D3)/($E$3*4*H138)</f>
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="M138">
+      <c r="M138" s="9"/>
+      <c r="N138">
         <f>G138^2</f>
         <v>4</v>
       </c>
-      <c r="N138">
-        <f>G138/O138</f>
+      <c r="O138">
+        <f>G138/P138</f>
         <v>0.57735026918962584</v>
       </c>
-      <c r="O138" s="5">
-        <f t="shared" ref="O138:O147" si="77">(3*M138/D3)^(1/2)</f>
+      <c r="P138" s="5">
+        <f t="shared" ref="P138:P147" si="77">(3*N138/D3)^(1/2)</f>
         <v>3.4641016151377544</v>
       </c>
-      <c r="P138" s="5">
-        <f t="shared" ref="P138:P147" si="78">(3/4)*((2*D3^(1/2))/(27^(1/2)*$E$3*M138^(1/2)))</f>
+      <c r="Q138" s="5">
+        <f t="shared" ref="Q138:Q147" si="78">(3/4)*((2*D3^(1/2))/(27^(1/2)*$E$3*N138^(1/2)))</f>
         <v>1.4433756729740644E-2</v>
       </c>
     </row>
-    <row r="139" spans="7:16">
+    <row r="139" spans="7:17">
       <c r="G139">
         <v>3.3</v>
       </c>
@@ -5974,24 +6077,25 @@
         <f t="shared" si="76"/>
         <v>1.8867924528301886E-2</v>
       </c>
-      <c r="M139">
-        <f t="shared" ref="M139:M147" si="80">M138+G139^2</f>
+      <c r="M139" s="9"/>
+      <c r="N139">
+        <f t="shared" ref="N139:N147" si="80">N138+G139^2</f>
         <v>14.889999999999999</v>
       </c>
-      <c r="N139">
-        <f t="shared" ref="N139:N147" si="81">G139/O139</f>
+      <c r="O139">
+        <f t="shared" ref="O139:O147" si="81">G139/P139</f>
         <v>0.69826610548066104</v>
       </c>
-      <c r="O139">
+      <c r="P139">
         <f t="shared" si="77"/>
         <v>4.7259919593668371</v>
       </c>
-      <c r="P139">
+      <c r="Q139">
         <f t="shared" si="78"/>
         <v>1.0579789476979712E-2</v>
       </c>
     </row>
-    <row r="140" spans="7:16">
+    <row r="140" spans="7:17">
       <c r="G140">
         <v>3.69</v>
       </c>
@@ -6011,24 +6115,25 @@
         <f t="shared" si="76"/>
         <v>2.5027808676307006E-2</v>
       </c>
-      <c r="M140">
+      <c r="M140" s="9"/>
+      <c r="N140">
         <f t="shared" si="80"/>
         <v>28.506099999999996</v>
       </c>
-      <c r="N140">
+      <c r="O140">
         <f t="shared" si="81"/>
         <v>0.69112637025787549</v>
       </c>
-      <c r="O140">
+      <c r="P140">
         <f t="shared" si="77"/>
         <v>5.3391104127935014</v>
       </c>
-      <c r="P140">
+      <c r="Q140">
         <f t="shared" si="78"/>
         <v>9.3648559655538678E-3</v>
       </c>
     </row>
-    <row r="141" spans="7:16">
+    <row r="141" spans="7:17">
       <c r="G141">
         <v>4.03</v>
       </c>
@@ -6048,24 +6153,25 @@
         <f t="shared" si="76"/>
         <v>3.0721966205837177E-2</v>
       </c>
-      <c r="M141">
+      <c r="M141" s="9"/>
+      <c r="N141">
         <f t="shared" si="80"/>
         <v>44.747</v>
       </c>
-      <c r="N141">
+      <c r="O141">
         <f t="shared" si="81"/>
         <v>0.69565266378459112</v>
       </c>
-      <c r="O141">
+      <c r="P141">
         <f t="shared" si="77"/>
         <v>5.7931209205401535</v>
       </c>
-      <c r="P141">
+      <c r="Q141">
         <f t="shared" si="78"/>
         <v>8.6309263496847522E-3</v>
       </c>
     </row>
-    <row r="142" spans="7:16">
+    <row r="142" spans="7:17">
       <c r="G142">
         <v>4.3</v>
       </c>
@@ -6085,24 +6191,25 @@
         <f t="shared" si="76"/>
         <v>3.6085450346420328E-2</v>
       </c>
-      <c r="M142">
+      <c r="M142" s="9"/>
+      <c r="N142">
         <f t="shared" si="80"/>
         <v>63.236999999999995</v>
       </c>
-      <c r="N142">
+      <c r="O142">
         <f t="shared" si="81"/>
         <v>0.69808322356386088</v>
       </c>
-      <c r="O142">
+      <c r="P142">
         <f t="shared" si="77"/>
         <v>6.1597240197917955</v>
       </c>
-      <c r="P142">
+      <c r="Q142">
         <f t="shared" si="78"/>
         <v>8.1172467856262896E-3</v>
       </c>
     </row>
-    <row r="143" spans="7:16">
+    <row r="143" spans="7:17">
       <c r="G143">
         <v>4.7</v>
       </c>
@@ -6122,24 +6229,25 @@
         <f t="shared" si="76"/>
         <v>4.0871934604904632E-2</v>
       </c>
-      <c r="M143">
+      <c r="M143" s="9"/>
+      <c r="N143">
         <f t="shared" si="80"/>
         <v>85.326999999999998</v>
       </c>
-      <c r="N143">
+      <c r="O143">
         <f t="shared" si="81"/>
         <v>0.71956431502003781</v>
       </c>
-      <c r="O143">
+      <c r="P143">
         <f t="shared" si="77"/>
         <v>6.5317302455015698</v>
       </c>
-      <c r="P143">
+      <c r="Q143">
         <f t="shared" si="78"/>
         <v>7.6549395214897623E-3</v>
       </c>
     </row>
-    <row r="144" spans="7:16">
+    <row r="144" spans="7:17">
       <c r="G144">
         <v>6.05</v>
       </c>
@@ -6159,24 +6267,25 @@
         <f t="shared" si="76"/>
         <v>4.3640897755610975E-2</v>
       </c>
-      <c r="M144">
+      <c r="M144" s="9"/>
+      <c r="N144">
         <f t="shared" si="80"/>
         <v>121.92949999999999</v>
       </c>
-      <c r="N144">
+      <c r="O144">
         <f t="shared" si="81"/>
         <v>0.83693045346583772</v>
       </c>
-      <c r="O144">
+      <c r="P144">
         <f t="shared" si="77"/>
         <v>7.2287965803444765</v>
       </c>
-      <c r="P144">
+      <c r="Q144">
         <f t="shared" si="78"/>
         <v>6.9167806071556842E-3</v>
       </c>
     </row>
-    <row r="145" spans="7:16">
+    <row r="145" spans="7:17">
       <c r="G145">
         <v>6.16</v>
       </c>
@@ -6196,24 +6305,25 @@
         <f t="shared" si="76"/>
         <v>4.6742623429739984E-2</v>
       </c>
-      <c r="M145">
+      <c r="M145" s="9"/>
+      <c r="N145">
         <f t="shared" si="80"/>
         <v>159.87509999999997</v>
       </c>
-      <c r="N145">
+      <c r="O145">
         <f t="shared" si="81"/>
         <v>0.79556315929010746</v>
       </c>
-      <c r="O145">
+      <c r="P145">
         <f t="shared" si="77"/>
         <v>7.7429427545346083</v>
       </c>
-      <c r="P145">
+      <c r="Q145">
         <f t="shared" si="78"/>
         <v>6.4574931760560663E-3</v>
       </c>
     </row>
-    <row r="146" spans="7:16">
+    <row r="146" spans="7:17">
       <c r="G146">
         <v>6.38</v>
       </c>
@@ -6233,24 +6343,25 @@
         <f t="shared" si="76"/>
         <v>4.9864565377985705E-2</v>
       </c>
-      <c r="M146">
+      <c r="M146" s="9"/>
+      <c r="N146">
         <f t="shared" si="80"/>
         <v>200.57949999999997</v>
       </c>
-      <c r="N146">
+      <c r="O146">
         <f t="shared" si="81"/>
         <v>0.78025764732937053</v>
       </c>
-      <c r="O146">
+      <c r="P146">
         <f t="shared" si="77"/>
         <v>8.1767862472571284</v>
       </c>
-      <c r="P146">
+      <c r="Q146">
         <f t="shared" si="78"/>
         <v>6.1148718442740639E-3</v>
       </c>
     </row>
-    <row r="147" spans="7:16">
+    <row r="147" spans="7:17">
       <c r="G147">
         <v>7</v>
       </c>
@@ -6271,24 +6382,25 @@
         <f t="shared" si="76"/>
         <v>5.2509976895610155E-2</v>
       </c>
-      <c r="M147">
+      <c r="M147" s="9"/>
+      <c r="N147">
         <f t="shared" si="80"/>
         <v>249.57949999999997</v>
       </c>
-      <c r="N147">
+      <c r="O147">
         <f t="shared" si="81"/>
         <v>0.8089710078088056</v>
       </c>
-      <c r="O147" s="11">
+      <c r="P147" s="11">
         <f t="shared" si="77"/>
         <v>8.6529676990036197</v>
       </c>
-      <c r="P147" s="11">
+      <c r="Q147" s="11">
         <f t="shared" si="78"/>
         <v>5.778364341491469E-3</v>
       </c>
     </row>
-    <row r="148" spans="7:16">
+    <row r="148" spans="7:17">
       <c r="J148" s="20">
         <v>1.5</v>
       </c>
@@ -6297,11 +6409,12 @@
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="O148" s="1">
+      <c r="M148" s="9"/>
+      <c r="P148" s="1">
         <v>1.5</v>
       </c>
     </row>
-    <row r="149" spans="7:16">
+    <row r="149" spans="7:17">
       <c r="J149" s="19">
         <v>2.5</v>
       </c>
@@ -6310,7 +6423,8 @@
         <f>1/(10*J149)-H138/(10*J149*J149)</f>
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="O149" s="1">
+      <c r="M149" s="9"/>
+      <c r="P149" s="1">
         <v>2.5</v>
       </c>
     </row>

</xml_diff>